<commit_message>
feat: change data excel url and shit
</commit_message>
<xml_diff>
--- a/data/new/3 . databersih- Rekap Surat Masuk dan Lowongan 2025.xlsx
+++ b/data/new/3 . databersih- Rekap Surat Masuk dan Lowongan 2025.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Allan\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Allan\Documents\bbpvp_tfidf\data\new\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{944E264F-5D60-4BD9-8DD9-8F0EC4F658E1}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97D8AA36-DBE0-421D-B27E-B30C7DA82CC4}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12375" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="949" uniqueCount="489">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1101" uniqueCount="613">
   <si>
     <t>REKRUTMEN PERUSAHAAN TAHUN 2025</t>
   </si>
@@ -1498,6 +1498,404 @@
   </si>
   <si>
     <t>Membantu teknisi AC dalam pemasangan dan perbaikan</t>
+  </si>
+  <si>
+    <t>Welder (Keiso)</t>
+  </si>
+  <si>
+    <t>sementara kosongkan</t>
+  </si>
+  <si>
+    <t>Welder (Keiso), (smakan dengan kolom B) jika mau coba cek ada di KBJI 2014 (optional aja dl)</t>
+  </si>
+  <si>
+    <t>Mampu membaca gambar teknik, memotong plat atau pipa besi menggunakan gerinda dan alat potong lainnya sesuai gambar teknis, melakukan pengelasan plat atau pipa besi dengan mesin las SMAW dan GMAW termasuk pekerjaan di ketinggian, merapikan hasil las sesuai standar kualitas, serta bekerja sesuai target dan membuat laporan pekerjaan harian</t>
+  </si>
+  <si>
+    <t>Civil Engineer (Keiso)</t>
+  </si>
+  <si>
+    <t>Civil Engineer</t>
+  </si>
+  <si>
+    <t>Bertanggung jawab dalam membuat dan merencanakan seluruh pekerjaan konstruksi, menyusun RAB dan timeline pelaksanaan, serta membuat gambar layout dan desain bangunan. Selain itu, memberikan rekomendasi rencana kegiatan konstruksi yang akan dilaksanakan serta mengevaluasi kegiatan konstruksi yang sedang berjalan. Melakukan koordinasi dengan departemen lain untuk mendukung kegiatan kerja, mengawasi pekerjaan (supervisi) serta penerapan K3. Melakukan evaluasi dan pembinaan terhadap tim di bawah tanggung jawabnya, mampu menerjemahkan keinginan atasan kepada departemen lain untuk kelancaran kegiatan kerja, serta menyusun laporan sesuai tugas dan tanggung jawab berdasarkan perintah atasan.</t>
+  </si>
+  <si>
+    <t>Electrical Engineers (Keiso)</t>
+  </si>
+  <si>
+    <t>Electrical Engineers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Melakukan identifikasi terhadap kebutuhan listrik perusahaan, merancang sistem dan produk listrik yang sesuai, serta menganalisis dan membaca spesifikasi dari gambar teknis elektrikal perusahaan. Selain itu, mempertimbangkan dan merekomendasikan solusi terbaik untuk meningkatkan efisiensi sistem elektrikal perusahaan.
+</t>
+  </si>
+  <si>
+    <t>Barista (Indomaret)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bertanggung jawab menyiapkan dan menyajikan minuman kopi maupun non-kopi sesuai SOP Point Coffee, memberikan pelayanan yang ramah, cepat, dan profesional kepada pelanggan, serta mengoperasikan dan merawat peralatan kopi dengan baik. Selain itu, menjaga kebersihan area bar, peralatan, dan lingkungan kerja, melakukan pengecekan stok bahan baku serta membantu proses penyiapan bahan, mematuhi standar kebersihan, keamanan, dan kualitas produk, serta mendukung kelancaran operasional outlet Point Coffee secara keseluruhan.
+</t>
+  </si>
+  <si>
+    <t>Steel Maintenance (Pako Group)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Melakukan pekerjaan perawatan dan perbaikan peralatan di area Utility, termasuk penggunaan gerinda, pengelasan, dan kikir, serta membantu perbaikan atau pembuatan komponen baja yang digunakan dalam proses produksi velg. Selain itu, melaksanakan pekerjaan bangku (bench work) untuk memperbaiki atau memodifikasi peralatan, menjaga peralatan kerja agar selalu dalam kondisi baik dan siap pakai, serta mematuhi prosedur keselamatan dan kesehatan kerja (K3) saat menggunakan peralatan dan mesin.
+</t>
+  </si>
+  <si>
+    <t>Engineering (Rechand)</t>
+  </si>
+  <si>
+    <t>Engineering</t>
+  </si>
+  <si>
+    <t>Bertanggung jawab melakukan instalasi, perawatan, dan perbaikan sistem kelistrikan sesuai standar perusahaan, termasuk melaksanakan pekerjaan service dan maintenance Air Conditioner (AC) sebagai prioritas. Selain itu, menganalisis dan menangani permasalahan teknis di lapangan, bekerja sama dengan tim untuk menyelesaikan pekerjaan secara efektif dan tepat waktu, serta menjaga kualitas hasil pekerjaan dan keselamatan kerja.</t>
+  </si>
+  <si>
+    <t>Venture Capital Officer (Madani)</t>
+  </si>
+  <si>
+    <t>Bertanggung jawab dalam menjalin dan membina hubungan baik dengan mitra, nasabah, serta seluruh pemangku kepentingan guna menjaga loyalitas dan memperluas peluang bisnis secara berkelanjutan. Memberikan layanan konsultasi yang solutif dengan merekomendasikan produk pembiayaan yang tepat sesuai kebutuhan nasabah, serta berkomitmen penuh dalam mencapai target penjualan yang telah ditetapkan perusahaan. Selain itu, aktif dalam memantau perkembangan pasar, mengelola administrasi pendukung secara akurat, serta memberikan pelayanan yang ramah dan profesional demi meningkatkan kepuasan nasabah dan mendukung pertumbuhan operasional bisnis secara keseluruhan.</t>
+  </si>
+  <si>
+    <t>Teknisi Pendingin (Malindo)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Melakukan inspeksi rutin serta pencatatan kondisi unit pendingin, mengidentifikasi penyebab kerusakan dan melakukan tindakan perbaikan yang diperlukan, serta mengisi dan memantau refrigeran sesuai standar kerja. Selain itu, menjaga kebersihan area kerja dan peralatan teknisi, melaporkan hasil pekerjaan serta temuan teknis kepada atasan, dan memastikan operasional mesin pendingin berjalan optimal tanpa mengganggu proses produksi.
+</t>
+  </si>
+  <si>
+    <t>Teknisi Listrik (Malindo)</t>
+  </si>
+  <si>
+    <t>Teknisi Listrik</t>
+  </si>
+  <si>
+    <t>Melakukan pengecekan rutin terhadap panel listrik dan instalasi untuk memastikan sistem kelistrikan berfungsi dengan baik dan aman. Menangani gangguan listrik secara cepat dan tepat guna meminimalkan downtime produksi. Melaksanakan perawatan preventif dan korektif pada sistem kelistrikan agar kinerja peralatan tetap optimal. Memastikan seluruh instalasi listrik telah sesuai dengan standar K3 serta SOP perusahaan yang berlaku. Menyusun laporan hasil pekerjaan dan aktivitas maintenance secara berkala sebagai bahan evaluasi. Selain itu, berkoordinasi dengan tim maintenance lainnya untuk mendukung perbaikan yang terpadu dan efektif.</t>
+  </si>
+  <si>
+    <t>Analis Lingkungan (TuvNord)</t>
+  </si>
+  <si>
+    <t>Melakukan persiapan sampel, monitoring, analisis, serta penelitian dan pengujian terhadap seluruh proses pengolahan limbah yang sedang berjalan guna memastikan efektivitas sistem pengolahan. Mendukung penuh kegiatan pengambilan sampel, analisis kualitas air, serta pengoperasian instrumen laboratorium lingkungan sesuai dengan standar teknis yang ditetapkan. Secara disiplin mencatat setiap penggunaan peralatan pada formulir yang tersedia serta melakukan pengawasan terhadap kondisi alat, termasuk melaporkan kerusakan, mengusulkan kebutuhan kalibrasi, servis, maupun penggantian suku cadang kepada atasan. Selain itu, bertanggung jawab dalam melakukan input data hasil analisis ke dalam sistem atau software setelah melalui proses review oleh Team Leader atau Supervisor untuk menjamin akurasi dan validitas data laporan.</t>
+  </si>
+  <si>
+    <t>Field Service Engineer (TuvNord)</t>
+  </si>
+  <si>
+    <t>Field Service Engineer</t>
+  </si>
+  <si>
+    <t>Melakukan pengecekan dan pengambilan sampel udara ambien serta melaksanakan pemantauan emisi udara dari sumber tidak bergerak secara akurat sesuai standar prosedur operasional. Mengelola kunjungan lokasi, menyusun jadwal monitoring yang terorganisir, serta melakukan supervisi langsung terhadap teknisi lapangan untuk memastikan kualitas kerja yang konsisten. Selain itu, menjalankan operasional lapangan secara menyeluruh, memberikan dukungan teknis yang diperlukan, serta menangani troubleshooting atas kendala peralatan atau teknis di lokasi guna menjamin kelancaran proses pengambilan data dan kepatuhan terhadap regulasi lingkungan yang berlaku.</t>
+  </si>
+  <si>
+    <t>Operator Bubut CNC dan Manual (Mardizu)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bertanggung jawab mengoperasikan mesin bubut CNC dan manual sesuai standar kerja, melakukan setting awal mesin sebelum proses produksi, serta melakukan troubleshooting apabila terjadi gangguan pada mesin. Selain itu, memastikan hasil pekerjaan sesuai dengan gambar teknik dan spesifikasi, melaksanakan perawatan harian (preventive maintenance) mesin bubut, serta menjaga kebersihan area kerja dan keselamatan kerja.
+</t>
+  </si>
+  <si>
+    <t>Teknisi AC Bus dan Refrigerator (KikiJaya)</t>
+  </si>
+  <si>
+    <t>Melakukan instalasi, perawatan, dan perbaikan AC bus serta unit refrigerator untuk memastikan sistem pendingin berfungsi secara optimal. Melaksanakan pengecekan sistem pendingin dan kelistrikan secara berkala guna mencegah terjadinya gangguan. Mengidentifikasi serta menangani permasalahan teknis pada AC dan refrigerator dengan cepat dan tepat. Memastikan seluruh unit beroperasi sesuai standar operasional yang telah ditetapkan. Dalam pelaksanaan pekerjaan, bekerja sama dengan tim di lapangan untuk menyelesaikan tugas secara efektif, serta selalu menjaga keselamatan kerja dan kebersihan area kerja.</t>
+  </si>
+  <si>
+    <t>Operator Produksi (UABS)</t>
+  </si>
+  <si>
+    <t>Melaksanakan proses produksi pada assembly line sesuai SOP serta mengoperasikan mesin dan peralatan produksi dengan aman. Menerapkan prinsip 5S di area kerja, melakukan inspeksi awal terhadap peralatan dan hasil produksi, serta menjaga kualitas produk sesuai standar perusahaan. Melaporkan kendala produksi kepada atasan guna memastikan kelancaran operasional.</t>
+  </si>
+  <si>
+    <t>QA Inspector Operator (UABS)</t>
+  </si>
+  <si>
+    <t>QA Inspector Operator</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Melakukan pemeriksaan kualitas produk Incoming (IQC) dan Outgoing (OQC) dengan menggunakan alat ukur seperti multimeter, calipers, charge/discharge tester, dan alat ukur lainnya, serta mencatat dan merekam data hasil inspeksi secara akurat. Selain itu, menyusun dan membuat laporan hasil inspeksi kualitas, memastikan produk yang dikirim sesuai dengan standar mutu yang ditetapkan, serta berkoordinasi dengan tim produksi terkait temuan kualitas.
+</t>
+  </si>
+  <si>
+    <t>Staff IT (Gemabangun)</t>
+  </si>
+  <si>
+    <t>Staff IT</t>
+  </si>
+  <si>
+    <t>Melakukan pemeliharaan sistem secara menyeluruh yang mencakup perangkat keras (hardware) dan perangkat lunak (software) guna memastikan sistem berjalan dengan optimal. Melaksanakan pemeliharaan infrastruktur jaringan serta aplikasi yang terkait untuk mendukung kelancaran operasional. Selain itu, melakukan troubleshooting terhadap permasalahan hardware dan software di sisi pengguna secara efisien, efektif, dan tepat waktu.</t>
+  </si>
+  <si>
+    <t>Operator Assembly (Gemabangun)</t>
+  </si>
+  <si>
+    <t>Operator Assembly</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Melaksanakan proses perakitan (assembly) komponen atau produk sesuai gambar teknik, SOP, dan standar kualitas perusahaan, serta memeriksa dan memastikan kualitas produk menggunakan alat ukur seperti jangka sorong, mikrometer, dan alat ukur lainnya. Selain itu, melakukan pengecekan dimensi, fungsi, dan visual produk hasil assembly, melaksanakan wiring panel sesuai instruksi kerja dan standar kelistrikan, serta membaca dan memahami rangkaian elektrikal dan gambar teknik. Mengidentifikasi serta melaporkan ketidaksesuaian (defect) produk kepada atasan, menjaga kebersihan area kerja dengan menerapkan prinsip 5S, mengoperasikan dan merawat peralatan kerja secara benar, serta mengisi dan melaporkan hasil pekerjaan sesuai form atau sistem yang berlaku.
+</t>
+  </si>
+  <si>
+    <t>Operator Produksi (Paragon Corp)</t>
+  </si>
+  <si>
+    <t>Melaksanakan proses produksi sesuai prosedur dan standar operasional perusahaan dengan mengoperasikan mesin produksi, conveyor, atau proses manual sesuai instruksi kerja. Melakukan aktivitas filling, packing, unboxing, dan proses produksi lainnya serta memastikan kualitas produk sesuai standar yang telah ditetapkan. Menjaga keselamatan kerja (K3) selama proses produksi berlangsung, melakukan pengecekan awal dan akhir terhadap hasil produksi, serta menjaga kebersihan area kerja dengan menerapkan prinsip 5S. Bekerja sama dengan tim untuk mencapai target produksi, melaporkan kendala atau ketidaksesuaian proses produksi kepada atasan, serta bersedia bekerja di lapangan dengan sistem shift.</t>
+  </si>
+  <si>
+    <t>Operator Welding Steelwork (PLP)</t>
+  </si>
+  <si>
+    <t>Operator Welding Steelwork</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Melaksanakan proses pengelasan material sesuai gambar teknik dan standar kerja dengan mengoperasikan mesin welding MIG dan TIG sesuai prosedur, termasuk pengelasan material aluminium tipis dengan ketebalan ± 2,0–4,0 mm. Selain itu, memastikan hasil pengelasan memenuhi standar kualitas dan keselamatan kerja, melakukan pengecekan visual serta perbaikan (repair weld) bila diperlukan, menjaga kebersihan area kerja dan peralatan welding, serta mematuhi prosedur K3 selama proses pengelasan.
+</t>
+  </si>
+  <si>
+    <t>Technician Mechanical Plant (Paragon Corp)</t>
+  </si>
+  <si>
+    <t>Melakukan genba ke lapangan untuk mengecek pelaksanaan pekerjaan repair dan maintenance secara langsung. Mengoordinasikan pekerjaan di lapangan bersama tukang, kenek, maupun vendor eksternal agar pekerjaan berjalan lancar. Memastikan seluruh pekerjaan yang dilakukan oleh tukang, kenek, dan vendor telah sesuai dengan instruksi kerja yang ditetapkan. Menyusun daftar material yang dibutuhkan untuk mendukung pekerjaan repair dan maintenance, serta membuat laporan hasil pekerjaan secara berkala kepada supervisor.</t>
+  </si>
+  <si>
+    <t>Staff Engineering Design &amp; Development (Pako Group)</t>
+  </si>
+  <si>
+    <t>Staff Engeering Design &amp; Development</t>
+  </si>
+  <si>
+    <t>Membuat Design Styling sebanyak 20 hingga 30 sketsa sebagai tahap awal penentuan konsep visual, serta melaksanakan pembuatan graphic prototype untuk menguji tampilan produk dalam Project Development. Memonitor perkembangan setiap tahapan proyek secara berkala guna memastikan kesesuaian rencana, serta melakukan kegiatan promosi dan branding untuk memperkuat identitas merek serta memenuhi kebutuhan komunikasi visual internal perusahaan.</t>
+  </si>
+  <si>
+    <t>Teknisi Maintenence (Excel Metal)</t>
+  </si>
+  <si>
+    <t>Teknisi Maintenence</t>
+  </si>
+  <si>
+    <t>Melakukan perawatan dan perbaikan mesin produksi serta peralatan pendukung untuk memastikan kelancaran proses operasional. Menangani instalasi dan perbaikan sistem kelistrikan mesin, serta melaksanakan preventive dan corrective maintenance secara berkala. Melakukan pengecekan arus listrik kuat dan instalasi listrik pabrik guna menjamin keamanan dan keandalan sistem. Mengidentifikasi serta menganalisis gangguan pada mesin dan sistem kerja untuk menemukan solusi yang tepat. Memastikan seluruh mesin dan peralatan beroperasi secara aman dan optimal, serta mencatat dan melaporkan seluruh aktivitas maintenance kepada atasan sebagai bahan evaluasi.</t>
+  </si>
+  <si>
+    <t>Technician Aftersales (Greenway)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Melakukan evaluasi ulang, diagnosa, dan perbaikan baterai kendaraan listrik yang mengalami kondisi abnormal, serta mengumpulkan, mengklasifikasikan, dan menganalisis permasalahan maintenance baterai aftersales. Selain itu, melakukan pencatatan data maintenance dan pelacakan baterai aftersales untuk memastikan proses penyelesaian berjalan dengan baik, memberikan feedback tepat waktu terkait isu produk bermasalah, mendukung analisis akar masalah (root cause analysis) serta mendorong perbaikan berkelanjutan. Melaksanakan tindak lanjut dan monitoring terhadap efektivitas hasil perbaikan yang telah diterapkan, serta berkoordinasi dengan tim terkait guna meningkatkan kualitas produk dan layanan aftersales.
+</t>
+  </si>
+  <si>
+    <t>Teknisi AC (Essanto)</t>
+  </si>
+  <si>
+    <t>Melakukan pekerjaan pemasangan dan perawatan AC untuk memastikan unit berfungsi dengan baik dan optimal. Menangani perbaikan AC apabila terjadi kerusakan, serta mampu menganalisis penyebab kerusakan AC secara tepat guna menentukan tindakan perbaikan yang sesuai.</t>
+  </si>
+  <si>
+    <t>Sales Enginering (Rechand)</t>
+  </si>
+  <si>
+    <t>Sales Enginering</t>
+  </si>
+  <si>
+    <t>Melakukan kunjungan rutin serta membina dan menjaga hubungan baik dengan customer untuk menjaga loyalitas dan kepercayaan. Menguasai product knowledge perusahaan secara mendalam guna memberikan solusi produk yang tepat sesuai kebutuhan, serta melakukan presentasi dan komunikasi produk dengan baik kepada customer. Selain itu, melakukan kontrol dan monitoring secara rutin terhadap hasil promosi dan penjualan yang sedang berjalan untuk memastikan efektivitas strategi yang diterapkan.</t>
+  </si>
+  <si>
+    <t>Teknisi Telekomunikasi (Pangestu)</t>
+  </si>
+  <si>
+    <t>Melaksanakan pekerjaan instalasi dan pemeliharaan jaringan telekomunikasi untuk memastikan sistem berjalan dengan baik. Mengikuti serta menjalani pelatihan yang diberikan oleh perusahaan guna meningkatkan keterampilan dan kompetensi kerja. Melaksanakan setiap pekerjaan sesuai dengan standar keselamatan dan prosedur kerja yang berlaku. Bekerja sama dalam tim untuk mencapai target pekerjaan yang telah ditetapkan, serta melaksanakan tugas di lapangan sesuai dengan penempatan wilayah kerja.</t>
+  </si>
+  <si>
+    <t>Teknisi Las (Prasetia)</t>
+  </si>
+  <si>
+    <t>Memahami teknik penarikan kabel fiber optic (FO) secara presisi dengan memperhatikan tensile strength (kekuatan tarik maksimal) guna mencegah kerusakan pada lapisan luar maupun inti kabel. Mampu mengoperasikan berbagai peralatan pendukung seperti fish tape (alat penarik kabel), cable roller (roda pemandu), hingga blowing machine (mesin tiup kabel) sesuai kebutuhan instalasi di lapangan. Selain itu, menguasai penggunaan alat teknis seperti OTDR untuk mendeteksi gangguan jaringan, power meter untuk mengukur kekuatan sinyal, serta splicer untuk melakukan penyambungan serat optik secara akurat.</t>
+  </si>
+  <si>
+    <t>Marketing Koordinator (Marsit Group)</t>
+  </si>
+  <si>
+    <t>Mengkoordinasikan dan mengontrol kinerja tim marketing lapangan serta melakukan monitoring terhadap pencapaian target dan aktivitas pemasaran secara intensif. Memberikan arahan taktis, evaluasi kerja, serta menyusun laporan kinerja tim secara berkala guna memastikan efektivitas strategi di lapangan. Selain itu, menjalin hubungan baik dengan mitra dan calon nasabah untuk memperluas jaringan serta mendukung penuh aktivitas pemasaran produk kredit, asuransi, maupun layanan keuangan lainnya demi mencapai pertumbuhan bisnis perusahaan.</t>
+  </si>
+  <si>
+    <t>Installer (Train4Best)</t>
+  </si>
+  <si>
+    <t>Melakukan instalasi perangkat telekomunikasi seluler sesuai dengan standar yang ditetapkan. Melaksanakan pekerjaan kelistrikan berdasarkan prosedur kerja yang berlaku untuk menjamin keamanan dan kualitas hasil pekerjaan. Melaksanakan tugas di lapangan, termasuk pekerjaan di ketinggian, dengan tetap mematuhi standar keselamatan dan kesehatan kerja (K3). Bekerja sama dengan tim secara efektif untuk menyelesaikan pekerjaan sesuai target yang telah ditentukan</t>
+  </si>
+  <si>
+    <t>Teknisi Repair Elektronik (Pangestu)</t>
+  </si>
+  <si>
+    <t>Melakukan perbaikan dan pengujian perangkat telekomunikasi, khususnya dalam menangani modul radio microwave, modul BTS (Base Transceiver Station), dan rectifier guna memastikan fungsionalitas perangkat kembali optimal. Melaksanakan seluruh rangkaian pekerjaan sesuai standar prosedur repair center dengan komitmen penuh untuk mencapai target waktu dan kualitas perbaikan yang ditetapkan. Selain itu, bersedia bekerja di luar jam kerja normal apabila dibutuhkan guna menangani kebutuhan perbaikan yang mendesak atau bersifat darurat.</t>
+  </si>
+  <si>
+    <t>Teknisi Mekatronik (Gemabangun)</t>
+  </si>
+  <si>
+    <t>Teknisi Mekatronik</t>
+  </si>
+  <si>
+    <t>Memeriksa dan memastikan kualitas produk sesuai dengan spesifikasi yang ditentukan menggunakan alat ukur yang relevan, seperti jangka sorong dan mikrometer, guna menjamin akurasi dimensi dan standar mutu. Selain itu, melakukan proses wiring mesin serta melaksanakan pengetesan sistem elektrikal, mekanikal, dan instalasi mesin secara menyeluruh di lokasi customer untuk memastikan seluruh fungsi operasional berjalan dengan optimal.</t>
+  </si>
+  <si>
+    <t>Teknisi Water Distribution dan Sewerage Staff (Jamabeka)</t>
+  </si>
+  <si>
+    <t>Teknisi Water Distribution dan Sewerage Staff</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Melaksanakan implementasi produk IoT yang mencakup checklist, monitoring, dan laporan pekerjaan harian, serta mengelola dan memastikan fungsionalitas sistem IoT melalui maintenance berkala. Selain itu, mengelola layanan managed service meliputi monitoring dashboard, dukungan terhadap anomali, dan mitigasi gangguan, serta mengelola sistem dokumentasi terstruktur untuk monitoring dan pembaruan catatan perbaikan.
+</t>
+  </si>
+  <si>
+    <t>Sales Consultant (Erablue)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Memasarkan dan menjual seluruh produk di Toko Erablue Elektronik, memandu pelanggan dalam memilih produk yang sesuai dengan kebutuhan, serta berorientasi pada pencapaian target penjualan bulanan.
+</t>
+  </si>
+  <si>
+    <t>Mobile App Developer (Redioro)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Merancang dan membuat tampilan antarmuka aplikasi, terbiasa menggunakan desain XML Android melalui Layout Editor, serta menggunakan Figma sebagai alat desain. Selain itu, terbiasa menggunakan Android Studio dengan bahasa Java dan memiliki pengalaman membuat aplikasi Android yang terhubung dengan REST API menggunakan Retrofit 2.
+</t>
+  </si>
+  <si>
+    <t>Desain 3D (Redioro)</t>
+  </si>
+  <si>
+    <t>Desain 3D</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Memahami penggunaan Blender atau software 3D sejenis, memiliki ketertarikan pada proses sculpting menggunakan Blender dan/atau Nomad Sculpt, serta berkesempatan menghasilkan produk melalui proses 3D printing dan laser.
+</t>
+  </si>
+  <si>
+    <t>Techician Operation (Summarecon)</t>
+  </si>
+  <si>
+    <t>Techician Operation</t>
+  </si>
+  <si>
+    <t>Memantau dan mengendalikan sistem teknis guna memastikan pemenuhan kebutuhan operasional mal, serta melaksanakan pemeliharaan rutin untuk mengoptimalkan kinerja sistem. Selain itu, berkolaborasi dengan tim lintas fungsi dalam mendukung tujuan operasional secara keseluruhan, melakukan perbaikan peralatan gedung agar berfungsi sesuai standar, memasang instalasi atau peralatan baru sesuai kebutuhan, mengajukan permintaan serta pengambilan suku cadang atau material dari gudang GA, serta memelihara seluruh peralatan, perlengkapan, dan area kerja agar tetap dalam kondisi baik.</t>
+  </si>
+  <si>
+    <t>Sales Consultant (Erajaya)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Melakukan penjualan produk kendaraan listrik (EV) XPENG kepada calon pelanggan dengan memberikan informasi produk secara lengkap, jelas, dan persuasif, serta melayani customer secara profesional dengan menjaga penampilan dan komunikasi yang baik. Selain itu, mengidentifikasi kebutuhan customer dan merekomendasikan produk yang sesuai, melakukan follow up prospek hingga proses penjualan selesai, menjaga serta membangun hubungan baik dengan customer, mencapai target penjualan yang ditetapkan perusahaan, serta mengikuti kegiatan promosi, pameran, dan event penjualan.
+</t>
+  </si>
+  <si>
+    <t>Safety, Health, and Environment Administrator (Paragorn Corp)</t>
+  </si>
+  <si>
+    <t>Safety, Health, and Environment Administrator</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mengelola administrasi dan dokumentasi terkait Keselamatan, Kesehatan Kerja, dan Lingkungan (K3L), serta membantu penerapan dan pemantauan program K3L di area kerja. Selain itu, menyusun, mengelola, dan memperbarui dokumen risiko kerja seperti Job Safety Analysis (JSA), mendukung kegiatan inspeksi K3, audit internal, dan pelaporan SHE, mengelola data dan laporan menggunakan software perkantoran, serta mendukung pengelolaan dan kesiapsiagaan tanggap darurat seperti APAR, P3K, tandu, dan eyewash. Berkoordinasi dengan tim terkait dalam pelaksanaan program SHE, serta melaksanakan pekerjaan administrasi dan kegiatan lapangan sesuai kebutuhan.
+</t>
+  </si>
+  <si>
+    <t>Operator Produksi Cleaning Service (Paragon Corp)</t>
+  </si>
+  <si>
+    <t>Operator Produksi Cleaning Service</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Melaksanakan kegiatan kebersihan di area produksi, fasilitas kerja, dan lingkungan perusahaan dengan menjaga kebersihan sesuai standar kebersihan dan keselamatan yang berlaku. Selain itu, melakukan pembersihan mesin, lantai, dinding, area umum, serta fasilitas pendukung menggunakan peralatan dan bahan pembersih sesuai prosedur, mendukung kelancaran proses produksi dengan menciptakan lingkungan kerja yang bersih dan aman, bekerja sama dengan tim sesuai jadwal yang ditentukan, melaporkan kondisi area kerja serta kebutuhan peralatan kepada atasan, dan bekerja di lapangan dengan sistem shift sesuai ketentuan perusahaan.
+</t>
+  </si>
+  <si>
+    <t>Kurir Sprinter (J&amp;T Express)</t>
+  </si>
+  <si>
+    <t>Kurir Sprinter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Melakukan pengantaran dan penjemputan paket ke alamat tujuan sesuai rute yang ditentukan, memastikan paket diterima pelanggan dengan aman, tepat waktu, dan dalam kondisi baik. Selain itu, mengoperasikan aplikasi pengiriman berbasis Android untuk memperbarui status paket, menjaga komunikasi yang baik dengan pelanggan dan tim operasional, bertanggung jawab atas kendaraan dan paket selama proses pengiriman, serta mematuhi SOP dan target pengiriman perusahaan.
+</t>
+  </si>
+  <si>
+    <t>Staff Accounting (Kanefusa)</t>
+  </si>
+  <si>
+    <t>Staff Accounting</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Melakukan pencatatan dan pengelolaan transaksi keuangan perusahaan, menyusun laporan keuangan secara berkala sesuai standar akuntansi, serta mengelola administrasi perpajakan dan dokumentasi keuangan. Selain itu, membantu proses audit internal maupun eksternal, mengoperasikan Microsoft Office untuk kebutuhan laporan dan administrasi, serta bekerja sesuai target dan mampu menangani tekanan pekerjaan.
+</t>
+  </si>
+  <si>
+    <t>Staff Engineering QC (Kanefusa)</t>
+  </si>
+  <si>
+    <t>Staff Engineering QC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Melakukan pengawasan dan pengendalian mutu (Quality Control) produk dengan melakukan pengecekan serta analisis kualitas sesuai standar perusahaan, menyusun laporan hasil inspeksi dan dokumentasi teknis, serta membantu proses perbaikan dan peningkatan kualitas produksi. Selain itu, mengoperasikan software pendukung seperti Microsoft Office dan AutoCAD, serta berkoordinasi dengan tim produksi dan engineering.
+</t>
+  </si>
+  <si>
+    <t>Operator Produksi (Kanefusa)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mengoperasikan mesin produksi sesuai SOP, melakukan pengecekan hasil produksi baik secara visual maupun menggunakan alat ukur, menjaga kualitas dan kuantitas hasil produksi, memastikan kebersihan serta keselamatan area kerja, dan melaporkan hasil kerja kepada atasan.
+</t>
+  </si>
+  <si>
+    <t>Teknisi Elektrik (Tenma)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Melakukan perawatan, perbaikan, dan troubleshooting sistem kelistrikan pada mesin produksi, termasuk menangani sistem pneumatik dan hidrolik pada mesin industri. Selain itu, melakukan pengecekan dan perbaikan sirkuit listrik, sakering, switch, transformer, serta motor AC/DC drive, membaca dan memahami skema kelistrikan dan diagram elektronik, melakukan pemrograman serta pengecekan PLC sesuai kebutuhan mesin, menangani perbaikan mesin Injection dan Molding, serta menyusun laporan hasil perawatan dan perbaikan mesin.
+</t>
+  </si>
+  <si>
+    <t>Teknisi HVAC (Adhi Trikarya)</t>
+  </si>
+  <si>
+    <t>Teknisi HVAC</t>
+  </si>
+  <si>
+    <t>Melaksanakan penugasan instalasi, pemeliharaan, dan perbaikan sistem MEP/HVAC, serta melakukan pengukuran hasil pekerjaan di lapangan yang meliputi kualitas, kuantitas, dan waktu pengujian.</t>
+  </si>
+  <si>
+    <t>Teknisi Repair Mould (Biggy)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bertanggung jawab langsung kepada Foreman Mold Repair atau Supervisor Technical dalam seluruh proses repair atau perbaikan molding, pembuatan jig accessories produksi, serta kegiatan lain yang berkaitan dengan proses produksi. Selain itu, memastikan kualitas molding setelah proses repair, pembuatan jig, dan optional yang dibutuhkan sesuai standar yang ditetapkan, mengontrol operasional molding yang sedang berjalan dalam produksi, serta melaksanakan SOP secara konsisten.
+</t>
+  </si>
+  <si>
+    <t>Teknisi Injection (Biggy)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bertanggung jawab langsung kepada Foreman Plan serta Foreman Injection dan Blow dalam seluruh kegiatan yang berkaitan dengan proses setting mesin produksi, memastikan kualitas dan kuantitas produk pada setiap mesin produksi sesuai standar yang ditetapkan. Selain itu, mengontrol operasional mesin produksi dan mould dengan melakukan perbaikan guna mencapai target mutu, waktu, efisiensi, dan produktivitas, melakukan evaluasi terhadap proses dan hasil produksi, serta menyusun laporan produksi per shift beserta hambatan yang dihadapi.
+</t>
+  </si>
+  <si>
+    <t>Operator CNC Milling (Biggy)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Melakukan pencarian titik referensi benda kerja sebelum menjalankan program pada mesin CNC, membuat program manual untuk pekerjaan sederhana tanpa menggunakan program CAM, serta melakukan input file NC dari komputer ke mesin CNC. Selain itu, membuat tool atau cutter single lip apabila diperlukan, melakukan pengecekan hasil kerja dengan mengacu pada gambar kerja yang dibuat oleh CAD Design, serta bertanggung jawab terhadap keamanan mesin selama masa pengoperasian agar tidak menyebabkan kerusakan pada benda kerja maupun mesin.
+</t>
+  </si>
+  <si>
+    <t>Operator Assy Mould (Biggy)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Melakukan pemeriksaan bagian-bagian mould dari segi dimensi dan mekanis dengan mengacu pada CAD drawing yang telah dibuat, serta melakukan pengecekan part yang telah diproduksi dengan membandingkannya terhadap gambar desain CAD. Selain itu, melaksanakan fitting test untuk setiap bagian mould yang menggunakan sistem sliding dan angular pin, melakukan pengecekan parting line produk pada mould, melakukan proses assembling mould, serta melakukan pengecekan sistem cooling baik pada mould baru maupun mould yang menjalani proses repair.
+</t>
+  </si>
+  <si>
+    <t>Project Manager Provider (STAFFINC)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mengelola dan mengoordinasikan proyek kerja sama dengan provider sesuai target dan timeline, menyusun perencanaan proyek, melakukan monitoring progres, serta mengevaluasi hasil pelaksanaan. Selain itu, melakukan komunikasi dan negosiasi dengan mitra atau provider, mengelola tim agar implementasi proyek berjalan efektif, menyusun laporan proyek dan presentasi menggunakan PowerPoint dan Excel, serta memastikan pencapaian target proyek dan penjualan sesuai ketentuan perusahaan.
+</t>
   </si>
 </sst>
 </file>
@@ -1507,11 +1905,18 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="d\ mmmm\ yyyy"/>
   </numFmts>
-  <fonts count="12">
+  <fonts count="13">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1584,7 +1989,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1633,8 +2038,14 @@
         <bgColor theme="0"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="7">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -1716,180 +2127,252 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="62">
+  <cellXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="15" fontId="7" fillId="0" borderId="5" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="15" fontId="8" fillId="0" borderId="5" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2134,26 +2617,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="42" customHeight="1">
-      <c r="A1" s="58" t="s">
+      <c r="A1" s="57" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="59"/>
-      <c r="C1" s="59"/>
-      <c r="D1" s="59"/>
-      <c r="E1" s="59"/>
-      <c r="F1" s="59"/>
-      <c r="G1" s="59"/>
-      <c r="H1" s="59"/>
-      <c r="I1" s="59"/>
-      <c r="J1" s="59"/>
-      <c r="K1" s="59"/>
-      <c r="L1" s="59"/>
-      <c r="M1" s="59"/>
-      <c r="N1" s="59"/>
-      <c r="O1" s="59"/>
-      <c r="P1" s="59"/>
-      <c r="Q1" s="59"/>
-      <c r="R1" s="60"/>
+      <c r="B1" s="58"/>
+      <c r="C1" s="58"/>
+      <c r="D1" s="58"/>
+      <c r="E1" s="58"/>
+      <c r="F1" s="58"/>
+      <c r="G1" s="58"/>
+      <c r="H1" s="58"/>
+      <c r="I1" s="58"/>
+      <c r="J1" s="58"/>
+      <c r="K1" s="58"/>
+      <c r="L1" s="58"/>
+      <c r="M1" s="58"/>
+      <c r="N1" s="58"/>
+      <c r="O1" s="58"/>
+      <c r="P1" s="58"/>
+      <c r="Q1" s="58"/>
+      <c r="R1" s="59"/>
     </row>
     <row r="2" spans="1:18" ht="45">
       <c r="A2" s="8" t="s">
@@ -2947,47 +3430,47 @@
       <c r="Q19" s="21"/>
       <c r="R19" s="21"/>
     </row>
-    <row r="20" spans="1:18" s="49" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A20" s="50">
-        <v>18</v>
-      </c>
-      <c r="B20" s="51" t="s">
-        <v>18</v>
-      </c>
-      <c r="C20" s="52">
+    <row r="20" spans="1:18" s="47" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A20" s="48">
+        <v>18</v>
+      </c>
+      <c r="B20" s="49" t="s">
+        <v>18</v>
+      </c>
+      <c r="C20" s="50">
         <v>45721</v>
       </c>
-      <c r="D20" s="51" t="s">
-        <v>18</v>
-      </c>
-      <c r="E20" s="53" t="s">
+      <c r="D20" s="49" t="s">
+        <v>18</v>
+      </c>
+      <c r="E20" s="51" t="s">
         <v>86</v>
       </c>
-      <c r="F20" s="50" t="s">
+      <c r="F20" s="48" t="s">
         <v>87</v>
       </c>
-      <c r="G20" s="50" t="s">
+      <c r="G20" s="48" t="s">
         <v>88</v>
       </c>
-      <c r="H20" s="54" t="s">
-        <v>18</v>
-      </c>
-      <c r="I20" s="54" t="s">
+      <c r="H20" s="52" t="s">
+        <v>18</v>
+      </c>
+      <c r="I20" s="52" t="s">
         <v>89</v>
       </c>
-      <c r="J20" s="55"/>
-      <c r="K20" s="55" t="s">
+      <c r="J20" s="53"/>
+      <c r="K20" s="53" t="s">
         <v>23</v>
       </c>
-      <c r="L20" s="46" t="s">
+      <c r="L20" s="44" t="s">
         <v>90</v>
       </c>
-      <c r="M20" s="53"/>
-      <c r="N20" s="53"/>
-      <c r="O20" s="53"/>
-      <c r="P20" s="53"/>
-      <c r="Q20" s="53"/>
-      <c r="R20" s="53"/>
+      <c r="M20" s="51"/>
+      <c r="N20" s="51"/>
+      <c r="O20" s="51"/>
+      <c r="P20" s="51"/>
+      <c r="Q20" s="51"/>
+      <c r="R20" s="51"/>
     </row>
     <row r="21" spans="1:18" ht="15.75" customHeight="1">
       <c r="A21" s="10">
@@ -5395,7 +5878,7 @@
       <c r="I101" s="6"/>
       <c r="J101" s="6"/>
       <c r="K101" s="6"/>
-      <c r="L101" s="36" t="s">
+      <c r="L101" s="34" t="s">
         <v>250</v>
       </c>
     </row>
@@ -14810,10 +15293,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F040F6F6-EB53-40F8-B637-6D3CBDAE75E2}">
-  <dimension ref="A1:F89"/>
+  <dimension ref="A1:F134"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="A85" sqref="A85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -14827,1719 +15310,2488 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15" customHeight="1">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="35" t="s">
         <v>274</v>
       </c>
-      <c r="B1" s="38" t="s">
+      <c r="B1" s="36" t="s">
         <v>251</v>
       </c>
-      <c r="C1" s="38" t="s">
+      <c r="C1" s="36" t="s">
         <v>252</v>
       </c>
-      <c r="D1" s="38" t="s">
+      <c r="D1" s="36" t="s">
         <v>253</v>
       </c>
-      <c r="E1" s="38" t="s">
+      <c r="E1" s="36" t="s">
         <v>254</v>
       </c>
-      <c r="F1" s="38" t="s">
+      <c r="F1" s="36" t="s">
         <v>255</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="15" customHeight="1">
-      <c r="A2" s="39">
+      <c r="A2" s="37">
         <v>1</v>
       </c>
-      <c r="B2" s="40" t="s">
+      <c r="B2" s="38" t="s">
         <v>24</v>
       </c>
-      <c r="C2" s="41">
+      <c r="C2" s="39">
         <v>3114</v>
       </c>
-      <c r="D2" s="40" t="s">
+      <c r="D2" s="38" t="s">
         <v>24</v>
       </c>
-      <c r="E2" s="40" t="s">
+      <c r="E2" s="38" t="s">
         <v>309</v>
       </c>
-      <c r="F2" s="40" t="s">
+      <c r="F2" s="38" t="s">
         <v>310</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="15" customHeight="1">
-      <c r="A3" s="39">
+      <c r="A3" s="37">
         <v>2</v>
       </c>
-      <c r="B3" s="40" t="s">
+      <c r="B3" s="38" t="s">
         <v>27</v>
       </c>
-      <c r="C3" s="41">
+      <c r="C3" s="39">
         <v>3322</v>
       </c>
-      <c r="D3" s="40" t="s">
+      <c r="D3" s="38" t="s">
         <v>256</v>
       </c>
-      <c r="E3" s="40" t="s">
+      <c r="E3" s="38" t="s">
         <v>257</v>
       </c>
-      <c r="F3" s="40" t="s">
+      <c r="F3" s="38" t="s">
         <v>311</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="15" customHeight="1">
-      <c r="A4" s="39">
+      <c r="A4" s="37">
         <v>3</v>
       </c>
-      <c r="B4" s="40" t="s">
+      <c r="B4" s="38" t="s">
         <v>30</v>
       </c>
-      <c r="C4" s="41">
+      <c r="C4" s="39">
         <v>4321</v>
       </c>
-      <c r="D4" s="40" t="s">
+      <c r="D4" s="38" t="s">
         <v>258</v>
       </c>
-      <c r="E4" s="40" t="s">
+      <c r="E4" s="38" t="s">
         <v>312</v>
       </c>
-      <c r="F4" s="40" t="s">
+      <c r="F4" s="38" t="s">
         <v>313</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="15" customHeight="1">
-      <c r="A5" s="39">
+      <c r="A5" s="37">
         <v>4</v>
       </c>
-      <c r="B5" s="40" t="s">
+      <c r="B5" s="38" t="s">
         <v>35</v>
       </c>
-      <c r="C5" s="41">
+      <c r="C5" s="39">
         <v>3322</v>
       </c>
-      <c r="D5" s="40" t="s">
+      <c r="D5" s="38" t="s">
         <v>256</v>
       </c>
-      <c r="E5" s="40" t="s">
+      <c r="E5" s="38" t="s">
         <v>314</v>
       </c>
-      <c r="F5" s="40" t="s">
+      <c r="F5" s="38" t="s">
         <v>315</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="15" customHeight="1">
-      <c r="A6" s="39">
+      <c r="A6" s="37">
         <v>5</v>
       </c>
-      <c r="B6" s="40" t="s">
+      <c r="B6" s="38" t="s">
         <v>41</v>
       </c>
-      <c r="C6" s="41">
+      <c r="C6" s="39">
         <v>2143</v>
       </c>
-      <c r="D6" s="40" t="s">
+      <c r="D6" s="38" t="s">
         <v>316</v>
       </c>
-      <c r="E6" s="40" t="s">
+      <c r="E6" s="38" t="s">
         <v>317</v>
       </c>
-      <c r="F6" s="40" t="s">
+      <c r="F6" s="38" t="s">
         <v>318</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="15" customHeight="1">
-      <c r="A7" s="39">
+      <c r="A7" s="37">
         <v>6</v>
       </c>
-      <c r="B7" s="40" t="s">
+      <c r="B7" s="38" t="s">
         <v>44</v>
       </c>
-      <c r="C7" s="41">
+      <c r="C7" s="39">
         <v>2149</v>
       </c>
-      <c r="D7" s="40" t="s">
+      <c r="D7" s="38" t="s">
         <v>319</v>
       </c>
-      <c r="E7" s="40" t="s">
+      <c r="E7" s="38" t="s">
         <v>320</v>
       </c>
-      <c r="F7" s="40" t="s">
+      <c r="F7" s="38" t="s">
         <v>321</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="15" customHeight="1">
-      <c r="A8" s="39">
+      <c r="A8" s="37">
         <v>7</v>
       </c>
-      <c r="B8" s="40" t="s">
+      <c r="B8" s="38" t="s">
         <v>47</v>
       </c>
-      <c r="C8" s="41">
+      <c r="C8" s="39">
         <v>4110</v>
       </c>
-      <c r="D8" s="40" t="s">
+      <c r="D8" s="38" t="s">
         <v>276</v>
       </c>
-      <c r="E8" s="40" t="s">
+      <c r="E8" s="38" t="s">
         <v>322</v>
       </c>
-      <c r="F8" s="40" t="s">
+      <c r="F8" s="38" t="s">
         <v>323</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="15" customHeight="1">
-      <c r="A9" s="39">
+      <c r="A9" s="37">
         <v>8</v>
       </c>
-      <c r="B9" s="40" t="s">
+      <c r="B9" s="38" t="s">
         <v>54</v>
       </c>
-      <c r="C9" s="41" t="s">
+      <c r="C9" s="39" t="s">
         <v>259</v>
       </c>
-      <c r="D9" s="40" t="s">
+      <c r="D9" s="38" t="s">
         <v>260</v>
       </c>
-      <c r="E9" s="40" t="s">
+      <c r="E9" s="38" t="s">
         <v>324</v>
       </c>
-      <c r="F9" s="40" t="s">
+      <c r="F9" s="38" t="s">
         <v>325</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="15" customHeight="1">
-      <c r="A10" s="39">
+      <c r="A10" s="37">
         <v>9</v>
       </c>
-      <c r="B10" s="40" t="s">
+      <c r="B10" s="38" t="s">
         <v>78</v>
       </c>
-      <c r="C10" s="41">
+      <c r="C10" s="39">
         <v>3118</v>
       </c>
-      <c r="D10" s="40" t="s">
+      <c r="D10" s="38" t="s">
         <v>288</v>
       </c>
-      <c r="E10" s="40" t="s">
+      <c r="E10" s="38" t="s">
         <v>326</v>
       </c>
-      <c r="F10" s="40" t="s">
+      <c r="F10" s="38" t="s">
         <v>327</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="15" customHeight="1">
-      <c r="A11" s="39">
+      <c r="A11" s="37">
         <v>10</v>
       </c>
-      <c r="B11" s="40" t="s">
+      <c r="B11" s="38" t="s">
         <v>66</v>
       </c>
-      <c r="C11" s="41">
+      <c r="C11" s="39">
         <v>7212</v>
       </c>
-      <c r="D11" s="40" t="s">
+      <c r="D11" s="38" t="s">
         <v>264</v>
       </c>
-      <c r="E11" s="40" t="s">
+      <c r="E11" s="38" t="s">
         <v>328</v>
       </c>
-      <c r="F11" s="40" t="s">
+      <c r="F11" s="38" t="s">
         <v>283</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="15" customHeight="1">
-      <c r="A12" s="39">
+      <c r="A12" s="37">
         <v>11</v>
       </c>
-      <c r="B12" s="40" t="s">
+      <c r="B12" s="38" t="s">
         <v>68</v>
       </c>
-      <c r="C12" s="41">
+      <c r="C12" s="39">
         <v>3115</v>
       </c>
-      <c r="D12" s="40" t="s">
+      <c r="D12" s="38" t="s">
         <v>294</v>
       </c>
-      <c r="E12" s="40" t="s">
+      <c r="E12" s="38" t="s">
         <v>329</v>
       </c>
-      <c r="F12" s="40" t="s">
+      <c r="F12" s="38" t="s">
         <v>306</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="15" customHeight="1">
-      <c r="A13" s="39">
+      <c r="A13" s="37">
         <v>12</v>
       </c>
-      <c r="B13" s="40" t="s">
+      <c r="B13" s="38" t="s">
         <v>72</v>
       </c>
-      <c r="C13" s="41">
+      <c r="C13" s="39">
         <v>3142</v>
       </c>
-      <c r="D13" s="40" t="s">
+      <c r="D13" s="38" t="s">
         <v>330</v>
       </c>
-      <c r="E13" s="40" t="s">
+      <c r="E13" s="38" t="s">
         <v>331</v>
       </c>
-      <c r="F13" s="40" t="s">
+      <c r="F13" s="38" t="s">
         <v>332</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="15" customHeight="1">
-      <c r="A14" s="39">
+      <c r="A14" s="37">
         <v>13</v>
       </c>
-      <c r="B14" s="40" t="s">
+      <c r="B14" s="38" t="s">
         <v>75</v>
       </c>
-      <c r="C14" s="41">
+      <c r="C14" s="39">
         <v>8321</v>
       </c>
-      <c r="D14" s="40" t="s">
+      <c r="D14" s="38" t="s">
         <v>333</v>
       </c>
-      <c r="E14" s="40" t="s">
+      <c r="E14" s="38" t="s">
         <v>334</v>
       </c>
-      <c r="F14" s="40" t="s">
+      <c r="F14" s="38" t="s">
         <v>275</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="15" customHeight="1">
-      <c r="A15" s="39">
+      <c r="A15" s="37">
         <v>14</v>
       </c>
-      <c r="B15" s="40" t="s">
+      <c r="B15" s="38" t="s">
         <v>83</v>
       </c>
-      <c r="C15" s="41">
+      <c r="C15" s="39">
         <v>3115</v>
       </c>
-      <c r="D15" s="40" t="s">
+      <c r="D15" s="38" t="s">
         <v>335</v>
       </c>
-      <c r="E15" s="40" t="s">
+      <c r="E15" s="38" t="s">
         <v>336</v>
       </c>
-      <c r="F15" s="40" t="s">
+      <c r="F15" s="38" t="s">
         <v>337</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="15" customHeight="1">
-      <c r="A16" s="39">
+      <c r="A16" s="37">
         <v>15</v>
       </c>
-      <c r="B16" s="40" t="s">
+      <c r="B16" s="38" t="s">
         <v>85</v>
       </c>
-      <c r="C16" s="41">
+      <c r="C16" s="39">
         <v>7412</v>
       </c>
-      <c r="D16" s="40" t="s">
+      <c r="D16" s="38" t="s">
         <v>338</v>
       </c>
-      <c r="E16" s="40" t="s">
+      <c r="E16" s="38" t="s">
         <v>339</v>
       </c>
-      <c r="F16" s="40" t="s">
+      <c r="F16" s="38" t="s">
         <v>340</v>
       </c>
     </row>
-    <row r="17" spans="1:6" s="49" customFormat="1" ht="15" customHeight="1">
-      <c r="A17" s="47">
+    <row r="17" spans="1:6" s="47" customFormat="1" ht="15" customHeight="1">
+      <c r="A17" s="45">
         <v>16</v>
       </c>
-      <c r="B17" s="56" t="s">
+      <c r="B17" s="54" t="s">
         <v>90</v>
       </c>
-      <c r="C17" s="57" t="s">
+      <c r="C17" s="55" t="s">
         <v>259</v>
       </c>
-      <c r="D17" s="56" t="s">
+      <c r="D17" s="54" t="s">
         <v>341</v>
       </c>
-      <c r="E17" s="61" t="s">
+      <c r="E17" s="56" t="s">
         <v>488</v>
       </c>
-      <c r="F17" s="48" t="s">
+      <c r="F17" s="46" t="s">
         <v>287</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="15" customHeight="1">
-      <c r="A18" s="39">
+      <c r="A18" s="37">
         <v>17</v>
       </c>
-      <c r="B18" s="40" t="s">
+      <c r="B18" s="38" t="s">
         <v>94</v>
       </c>
-      <c r="C18" s="41">
+      <c r="C18" s="39">
         <v>3114</v>
       </c>
-      <c r="D18" s="40" t="s">
+      <c r="D18" s="38" t="s">
         <v>342</v>
       </c>
-      <c r="E18" s="40" t="s">
+      <c r="E18" s="38" t="s">
         <v>343</v>
       </c>
-      <c r="F18" s="40" t="s">
+      <c r="F18" s="38" t="s">
         <v>344</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="15" customHeight="1">
-      <c r="A19" s="39">
-        <v>18</v>
-      </c>
-      <c r="B19" s="40" t="s">
+      <c r="A19" s="37">
+        <v>18</v>
+      </c>
+      <c r="B19" s="38" t="s">
         <v>96</v>
       </c>
-      <c r="C19" s="41" t="s">
+      <c r="C19" s="39" t="s">
         <v>259</v>
       </c>
-      <c r="D19" s="40" t="s">
+      <c r="D19" s="38" t="s">
         <v>138</v>
       </c>
-      <c r="E19" s="40" t="s">
+      <c r="E19" s="38" t="s">
         <v>345</v>
       </c>
-      <c r="F19" s="40" t="s">
+      <c r="F19" s="38" t="s">
         <v>346</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="15" customHeight="1">
-      <c r="A20" s="39">
+      <c r="A20" s="37">
         <v>19</v>
       </c>
-      <c r="B20" s="40" t="s">
+      <c r="B20" s="38" t="s">
         <v>97</v>
       </c>
-      <c r="C20" s="41">
+      <c r="C20" s="39">
         <v>4110</v>
       </c>
-      <c r="D20" s="40" t="s">
+      <c r="D20" s="38" t="s">
         <v>347</v>
       </c>
-      <c r="E20" s="40" t="s">
+      <c r="E20" s="38" t="s">
         <v>348</v>
       </c>
-      <c r="F20" s="40" t="s">
+      <c r="F20" s="38" t="s">
         <v>349</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="15" customHeight="1">
-      <c r="A21" s="39">
+      <c r="A21" s="37">
         <v>20</v>
       </c>
-      <c r="B21" s="40" t="s">
+      <c r="B21" s="38" t="s">
         <v>99</v>
       </c>
-      <c r="C21" s="41">
+      <c r="C21" s="39">
         <v>7412</v>
       </c>
-      <c r="D21" s="40" t="s">
+      <c r="D21" s="38" t="s">
         <v>261</v>
       </c>
-      <c r="E21" s="40" t="s">
+      <c r="E21" s="38" t="s">
         <v>350</v>
       </c>
-      <c r="F21" s="40" t="s">
+      <c r="F21" s="38" t="s">
         <v>351</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="15" customHeight="1">
-      <c r="A22" s="39">
+      <c r="A22" s="37">
         <v>21</v>
       </c>
-      <c r="B22" s="40" t="s">
+      <c r="B22" s="38" t="s">
         <v>352</v>
       </c>
-      <c r="C22" s="41">
+      <c r="C22" s="39">
         <v>3322</v>
       </c>
-      <c r="D22" s="40" t="s">
+      <c r="D22" s="38" t="s">
         <v>256</v>
       </c>
-      <c r="E22" s="40" t="s">
+      <c r="E22" s="38" t="s">
         <v>353</v>
       </c>
-      <c r="F22" s="40" t="s">
+      <c r="F22" s="38" t="s">
         <v>354</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="15" customHeight="1">
-      <c r="A23" s="39">
+      <c r="A23" s="37">
         <v>22</v>
       </c>
-      <c r="B23" s="40" t="s">
+      <c r="B23" s="38" t="s">
         <v>69</v>
       </c>
-      <c r="C23" s="41">
+      <c r="C23" s="39">
         <v>8131</v>
       </c>
-      <c r="D23" s="40" t="s">
+      <c r="D23" s="38" t="s">
         <v>130</v>
       </c>
-      <c r="E23" s="40" t="s">
+      <c r="E23" s="38" t="s">
         <v>355</v>
       </c>
-      <c r="F23" s="40" t="s">
+      <c r="F23" s="38" t="s">
         <v>356</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="15" customHeight="1">
-      <c r="A24" s="39">
+      <c r="A24" s="37">
         <v>23</v>
       </c>
-      <c r="B24" s="40" t="s">
+      <c r="B24" s="38" t="s">
         <v>357</v>
       </c>
-      <c r="C24" s="41">
+      <c r="C24" s="39">
         <v>3115</v>
       </c>
-      <c r="D24" s="40" t="s">
+      <c r="D24" s="38" t="s">
         <v>294</v>
       </c>
-      <c r="E24" s="40" t="s">
+      <c r="E24" s="38" t="s">
         <v>358</v>
       </c>
-      <c r="F24" s="40" t="s">
+      <c r="F24" s="38" t="s">
         <v>359</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="15" customHeight="1">
-      <c r="A25" s="39">
+      <c r="A25" s="37">
         <v>24</v>
       </c>
-      <c r="B25" s="40" t="s">
+      <c r="B25" s="38" t="s">
         <v>113</v>
       </c>
-      <c r="C25" s="41">
+      <c r="C25" s="39">
         <v>7223</v>
       </c>
-      <c r="D25" s="40" t="s">
+      <c r="D25" s="38" t="s">
         <v>262</v>
       </c>
-      <c r="E25" s="40" t="s">
+      <c r="E25" s="38" t="s">
         <v>360</v>
       </c>
-      <c r="F25" s="40" t="s">
+      <c r="F25" s="38" t="s">
         <v>361</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="15" customHeight="1">
-      <c r="A26" s="39">
+      <c r="A26" s="37">
         <v>25</v>
       </c>
-      <c r="B26" s="40" t="s">
+      <c r="B26" s="38" t="s">
         <v>117</v>
       </c>
-      <c r="C26" s="41">
+      <c r="C26" s="39">
         <v>7422</v>
       </c>
-      <c r="D26" s="40" t="s">
+      <c r="D26" s="38" t="s">
         <v>362</v>
       </c>
-      <c r="E26" s="40" t="s">
+      <c r="E26" s="38" t="s">
         <v>277</v>
       </c>
-      <c r="F26" s="40" t="s">
+      <c r="F26" s="38" t="s">
         <v>363</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="15" customHeight="1">
-      <c r="A27" s="39">
+      <c r="A27" s="37">
         <v>26</v>
       </c>
-      <c r="B27" s="40" t="s">
+      <c r="B27" s="38" t="s">
         <v>119</v>
       </c>
-      <c r="C27" s="41">
+      <c r="C27" s="39">
         <v>2413</v>
       </c>
-      <c r="D27" s="40" t="s">
+      <c r="D27" s="38" t="s">
         <v>364</v>
       </c>
-      <c r="E27" s="40" t="s">
+      <c r="E27" s="38" t="s">
         <v>365</v>
       </c>
-      <c r="F27" s="40" t="s">
+      <c r="F27" s="38" t="s">
         <v>366</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="15" customHeight="1">
-      <c r="A28" s="39">
+      <c r="A28" s="37">
         <v>27</v>
       </c>
-      <c r="B28" s="40" t="s">
+      <c r="B28" s="38" t="s">
         <v>367</v>
       </c>
-      <c r="C28" s="41" t="s">
+      <c r="C28" s="39" t="s">
         <v>259</v>
       </c>
-      <c r="D28" s="40" t="s">
+      <c r="D28" s="38" t="s">
         <v>138</v>
       </c>
-      <c r="E28" s="40" t="s">
+      <c r="E28" s="38" t="s">
         <v>368</v>
       </c>
-      <c r="F28" s="40" t="s">
+      <c r="F28" s="38" t="s">
         <v>369</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="15" customHeight="1">
-      <c r="A29" s="39">
+      <c r="A29" s="37">
         <v>28</v>
       </c>
-      <c r="B29" s="40" t="s">
+      <c r="B29" s="38" t="s">
         <v>126</v>
       </c>
-      <c r="C29" s="41">
+      <c r="C29" s="39">
         <v>7223</v>
       </c>
-      <c r="D29" s="40" t="s">
+      <c r="D29" s="38" t="s">
         <v>370</v>
       </c>
-      <c r="E29" s="40" t="s">
+      <c r="E29" s="38" t="s">
         <v>371</v>
       </c>
-      <c r="F29" s="40" t="s">
+      <c r="F29" s="38" t="s">
         <v>372</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="15" customHeight="1">
-      <c r="A30" s="39">
+      <c r="A30" s="37">
         <v>29</v>
       </c>
-      <c r="B30" s="40" t="s">
+      <c r="B30" s="38" t="s">
         <v>279</v>
       </c>
-      <c r="C30" s="41">
+      <c r="C30" s="39">
         <v>2132</v>
       </c>
-      <c r="D30" s="40" t="s">
+      <c r="D30" s="38" t="s">
         <v>280</v>
       </c>
-      <c r="E30" s="40" t="s">
+      <c r="E30" s="38" t="s">
         <v>373</v>
       </c>
-      <c r="F30" s="40" t="s">
+      <c r="F30" s="38" t="s">
         <v>374</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="15" customHeight="1">
-      <c r="A31" s="39">
+      <c r="A31" s="37">
         <v>30</v>
       </c>
-      <c r="B31" s="40" t="s">
+      <c r="B31" s="38" t="s">
         <v>130</v>
       </c>
-      <c r="C31" s="41">
+      <c r="C31" s="39">
         <v>8131</v>
       </c>
-      <c r="D31" s="40" t="s">
+      <c r="D31" s="38" t="s">
         <v>69</v>
       </c>
-      <c r="E31" s="40" t="s">
+      <c r="E31" s="38" t="s">
         <v>375</v>
       </c>
-      <c r="F31" s="40" t="s">
+      <c r="F31" s="38" t="s">
         <v>376</v>
       </c>
     </row>
     <row r="32" spans="1:6">
-      <c r="A32" s="39">
+      <c r="A32" s="37">
         <v>31</v>
       </c>
-      <c r="B32" s="40" t="s">
+      <c r="B32" s="38" t="s">
         <v>134</v>
       </c>
-      <c r="C32" s="41">
+      <c r="C32" s="39">
         <v>3132</v>
       </c>
-      <c r="D32" s="40" t="s">
+      <c r="D32" s="38" t="s">
         <v>278</v>
       </c>
-      <c r="E32" s="40" t="s">
+      <c r="E32" s="38" t="s">
         <v>377</v>
       </c>
-      <c r="F32" s="40" t="s">
+      <c r="F32" s="38" t="s">
         <v>378</v>
       </c>
     </row>
-    <row r="33" spans="1:6" s="45" customFormat="1">
-      <c r="A33" s="42">
+    <row r="33" spans="1:6" s="43" customFormat="1">
+      <c r="A33" s="40">
         <v>32</v>
       </c>
-      <c r="B33" s="43" t="s">
+      <c r="B33" s="41" t="s">
         <v>138</v>
       </c>
-      <c r="C33" s="44" t="s">
+      <c r="C33" s="42" t="s">
         <v>259</v>
       </c>
-      <c r="D33" s="43" t="s">
+      <c r="D33" s="41" t="s">
         <v>138</v>
       </c>
-      <c r="E33" s="43" t="s">
+      <c r="E33" s="41" t="s">
         <v>379</v>
       </c>
-      <c r="F33" s="43" t="s">
+      <c r="F33" s="41" t="s">
         <v>380</v>
       </c>
     </row>
     <row r="34" spans="1:6">
-      <c r="A34" s="39">
+      <c r="A34" s="37">
         <v>33</v>
       </c>
-      <c r="B34" s="40" t="s">
+      <c r="B34" s="38" t="s">
         <v>143</v>
       </c>
-      <c r="C34" s="41">
+      <c r="C34" s="39">
         <v>3322</v>
       </c>
-      <c r="D34" s="40" t="s">
+      <c r="D34" s="38" t="s">
         <v>281</v>
       </c>
-      <c r="E34" s="40" t="s">
+      <c r="E34" s="38" t="s">
         <v>381</v>
       </c>
-      <c r="F34" s="40" t="s">
+      <c r="F34" s="38" t="s">
         <v>382</v>
       </c>
     </row>
     <row r="35" spans="1:6">
-      <c r="A35" s="39">
+      <c r="A35" s="37">
         <v>34</v>
       </c>
-      <c r="B35" s="40" t="s">
+      <c r="B35" s="38" t="s">
         <v>148</v>
       </c>
-      <c r="C35" s="41">
+      <c r="C35" s="39">
         <v>2149</v>
       </c>
-      <c r="D35" s="40" t="s">
+      <c r="D35" s="38" t="s">
         <v>383</v>
       </c>
-      <c r="E35" s="40" t="s">
+      <c r="E35" s="38" t="s">
         <v>384</v>
       </c>
-      <c r="F35" s="40" t="s">
+      <c r="F35" s="38" t="s">
         <v>385</v>
       </c>
     </row>
-    <row r="36" spans="1:6" s="45" customFormat="1">
-      <c r="A36" s="42">
+    <row r="36" spans="1:6" s="43" customFormat="1">
+      <c r="A36" s="40">
         <v>35</v>
       </c>
-      <c r="B36" s="43" t="s">
+      <c r="B36" s="41" t="s">
         <v>151</v>
       </c>
-      <c r="C36" s="44">
+      <c r="C36" s="42">
         <v>2512</v>
       </c>
-      <c r="D36" s="43" t="s">
+      <c r="D36" s="41" t="s">
         <v>282</v>
       </c>
-      <c r="E36" s="43" t="s">
+      <c r="E36" s="41" t="s">
         <v>386</v>
       </c>
-      <c r="F36" s="43" t="s">
+      <c r="F36" s="41" t="s">
         <v>387</v>
       </c>
     </row>
     <row r="37" spans="1:6">
-      <c r="A37" s="39">
+      <c r="A37" s="37">
         <v>36</v>
       </c>
-      <c r="B37" s="40" t="s">
+      <c r="B37" s="38" t="s">
         <v>154</v>
       </c>
-      <c r="C37" s="41">
+      <c r="C37" s="39">
         <v>7412</v>
       </c>
-      <c r="D37" s="40" t="s">
+      <c r="D37" s="38" t="s">
         <v>388</v>
       </c>
-      <c r="E37" s="40" t="s">
+      <c r="E37" s="38" t="s">
         <v>389</v>
       </c>
-      <c r="F37" s="40" t="s">
+      <c r="F37" s="38" t="s">
         <v>390</v>
       </c>
     </row>
-    <row r="38" spans="1:6" s="45" customFormat="1">
-      <c r="A38" s="42">
+    <row r="38" spans="1:6" s="43" customFormat="1">
+      <c r="A38" s="40">
         <v>37</v>
       </c>
-      <c r="B38" s="43" t="s">
+      <c r="B38" s="41" t="s">
         <v>159</v>
       </c>
-      <c r="C38" s="44">
+      <c r="C38" s="42">
         <v>7212</v>
       </c>
-      <c r="D38" s="43" t="s">
+      <c r="D38" s="41" t="s">
         <v>199</v>
       </c>
-      <c r="E38" s="43" t="s">
+      <c r="E38" s="41" t="s">
         <v>391</v>
       </c>
-      <c r="F38" s="43" t="s">
+      <c r="F38" s="41" t="s">
         <v>392</v>
       </c>
     </row>
     <row r="39" spans="1:6">
-      <c r="A39" s="39">
+      <c r="A39" s="37">
         <v>38</v>
       </c>
-      <c r="B39" s="40" t="s">
+      <c r="B39" s="38" t="s">
         <v>162</v>
       </c>
-      <c r="C39" s="41">
+      <c r="C39" s="39">
         <v>1420</v>
       </c>
-      <c r="D39" s="40" t="s">
+      <c r="D39" s="38" t="s">
         <v>393</v>
       </c>
-      <c r="E39" s="40" t="s">
+      <c r="E39" s="38" t="s">
         <v>394</v>
       </c>
-      <c r="F39" s="40" t="s">
+      <c r="F39" s="38" t="s">
         <v>395</v>
       </c>
     </row>
     <row r="40" spans="1:6">
-      <c r="A40" s="39">
+      <c r="A40" s="37">
         <v>39</v>
       </c>
-      <c r="B40" s="40" t="s">
+      <c r="B40" s="38" t="s">
         <v>164</v>
       </c>
-      <c r="C40" s="41" t="s">
+      <c r="C40" s="39" t="s">
         <v>259</v>
       </c>
-      <c r="D40" s="40" t="s">
+      <c r="D40" s="38" t="s">
         <v>138</v>
       </c>
-      <c r="E40" s="40" t="s">
+      <c r="E40" s="38" t="s">
         <v>396</v>
       </c>
-      <c r="F40" s="40" t="s">
+      <c r="F40" s="38" t="s">
         <v>397</v>
       </c>
     </row>
     <row r="41" spans="1:6">
-      <c r="A41" s="39">
+      <c r="A41" s="37">
         <v>40</v>
       </c>
-      <c r="B41" s="40" t="s">
+      <c r="B41" s="38" t="s">
         <v>168</v>
       </c>
-      <c r="C41" s="41">
+      <c r="C41" s="39">
         <v>2431</v>
       </c>
-      <c r="D41" s="40" t="s">
+      <c r="D41" s="38" t="s">
         <v>284</v>
       </c>
-      <c r="E41" s="40" t="s">
+      <c r="E41" s="38" t="s">
         <v>398</v>
       </c>
-      <c r="F41" s="40" t="s">
+      <c r="F41" s="38" t="s">
         <v>399</v>
       </c>
     </row>
     <row r="42" spans="1:6">
-      <c r="A42" s="39">
+      <c r="A42" s="37">
         <v>41</v>
       </c>
-      <c r="B42" s="40" t="s">
+      <c r="B42" s="38" t="s">
         <v>400</v>
       </c>
-      <c r="C42" s="41">
+      <c r="C42" s="39">
         <v>3114</v>
       </c>
-      <c r="D42" s="40" t="s">
+      <c r="D42" s="38" t="s">
         <v>24</v>
       </c>
-      <c r="E42" s="40" t="s">
+      <c r="E42" s="38" t="s">
         <v>401</v>
       </c>
-      <c r="F42" s="40" t="s">
+      <c r="F42" s="38" t="s">
         <v>402</v>
       </c>
     </row>
-    <row r="43" spans="1:6" s="45" customFormat="1">
-      <c r="A43" s="42">
+    <row r="43" spans="1:6" s="43" customFormat="1">
+      <c r="A43" s="40">
         <v>42</v>
       </c>
-      <c r="B43" s="43" t="s">
+      <c r="B43" s="41" t="s">
         <v>177</v>
       </c>
-      <c r="C43" s="44">
+      <c r="C43" s="42">
         <v>7422</v>
       </c>
-      <c r="D43" s="43" t="s">
+      <c r="D43" s="41" t="s">
         <v>177</v>
       </c>
-      <c r="E43" s="43" t="s">
+      <c r="E43" s="41" t="s">
         <v>403</v>
       </c>
-      <c r="F43" s="43" t="s">
+      <c r="F43" s="41" t="s">
         <v>271</v>
       </c>
     </row>
     <row r="44" spans="1:6">
-      <c r="A44" s="39">
+      <c r="A44" s="37">
         <v>43</v>
       </c>
-      <c r="B44" s="40" t="s">
+      <c r="B44" s="38" t="s">
         <v>179</v>
       </c>
-      <c r="C44" s="41">
+      <c r="C44" s="39">
         <v>3139</v>
       </c>
-      <c r="D44" s="40" t="s">
+      <c r="D44" s="38" t="s">
         <v>404</v>
       </c>
-      <c r="E44" s="40" t="s">
+      <c r="E44" s="38" t="s">
         <v>405</v>
       </c>
-      <c r="F44" s="40" t="s">
+      <c r="F44" s="38" t="s">
         <v>406</v>
       </c>
     </row>
-    <row r="45" spans="1:6" s="45" customFormat="1">
-      <c r="A45" s="42">
+    <row r="45" spans="1:6" s="43" customFormat="1">
+      <c r="A45" s="40">
         <v>44</v>
       </c>
-      <c r="B45" s="43" t="s">
+      <c r="B45" s="41" t="s">
         <v>189</v>
       </c>
-      <c r="C45" s="44">
+      <c r="C45" s="42">
         <v>5132</v>
       </c>
-      <c r="D45" s="43" t="s">
+      <c r="D45" s="41" t="s">
         <v>189</v>
       </c>
-      <c r="E45" s="43" t="s">
+      <c r="E45" s="41" t="s">
         <v>407</v>
       </c>
-      <c r="F45" s="43" t="s">
+      <c r="F45" s="41" t="s">
         <v>269</v>
       </c>
     </row>
     <row r="46" spans="1:6">
-      <c r="A46" s="39">
+      <c r="A46" s="37">
         <v>45</v>
       </c>
-      <c r="B46" s="40" t="s">
+      <c r="B46" s="38" t="s">
         <v>191</v>
       </c>
-      <c r="C46" s="41">
+      <c r="C46" s="39">
         <v>2424</v>
       </c>
-      <c r="D46" s="40" t="s">
+      <c r="D46" s="38" t="s">
         <v>408</v>
       </c>
-      <c r="E46" s="40" t="s">
+      <c r="E46" s="38" t="s">
         <v>409</v>
       </c>
-      <c r="F46" s="40" t="s">
+      <c r="F46" s="38" t="s">
         <v>285</v>
       </c>
     </row>
-    <row r="47" spans="1:6" s="45" customFormat="1">
-      <c r="A47" s="42">
+    <row r="47" spans="1:6" s="43" customFormat="1">
+      <c r="A47" s="40">
         <v>46</v>
       </c>
-      <c r="B47" s="43" t="s">
+      <c r="B47" s="41" t="s">
         <v>196</v>
       </c>
-      <c r="C47" s="44" t="s">
+      <c r="C47" s="42" t="s">
         <v>259</v>
       </c>
-      <c r="D47" s="43" t="s">
+      <c r="D47" s="41" t="s">
         <v>341</v>
       </c>
-      <c r="E47" s="43" t="s">
+      <c r="E47" s="41" t="s">
         <v>286</v>
       </c>
-      <c r="F47" s="43" t="s">
+      <c r="F47" s="41" t="s">
         <v>287</v>
       </c>
     </row>
     <row r="48" spans="1:6">
-      <c r="A48" s="39">
+      <c r="A48" s="37">
         <v>47</v>
       </c>
-      <c r="B48" s="40" t="s">
+      <c r="B48" s="38" t="s">
         <v>199</v>
       </c>
-      <c r="C48" s="41">
+      <c r="C48" s="39">
         <v>7212</v>
       </c>
-      <c r="D48" s="40" t="s">
+      <c r="D48" s="38" t="s">
         <v>264</v>
       </c>
-      <c r="E48" s="40" t="s">
+      <c r="E48" s="38" t="s">
         <v>410</v>
       </c>
-      <c r="F48" s="40" t="s">
+      <c r="F48" s="38" t="s">
         <v>283</v>
       </c>
     </row>
     <row r="49" spans="1:6">
-      <c r="A49" s="39">
+      <c r="A49" s="37">
         <v>48</v>
       </c>
-      <c r="B49" s="40" t="s">
+      <c r="B49" s="38" t="s">
         <v>411</v>
       </c>
-      <c r="C49" s="41">
+      <c r="C49" s="39">
         <v>2431</v>
       </c>
-      <c r="D49" s="40" t="s">
+      <c r="D49" s="38" t="s">
         <v>412</v>
       </c>
-      <c r="E49" s="40" t="s">
+      <c r="E49" s="38" t="s">
         <v>413</v>
       </c>
-      <c r="F49" s="40" t="s">
+      <c r="F49" s="38" t="s">
         <v>414</v>
       </c>
     </row>
     <row r="50" spans="1:6">
-      <c r="A50" s="39">
+      <c r="A50" s="37">
         <v>49</v>
       </c>
-      <c r="B50" s="40" t="s">
+      <c r="B50" s="38" t="s">
         <v>204</v>
       </c>
-      <c r="C50" s="41">
+      <c r="C50" s="39">
         <v>3119</v>
       </c>
-      <c r="D50" s="40" t="s">
+      <c r="D50" s="38" t="s">
         <v>267</v>
       </c>
-      <c r="E50" s="40" t="s">
+      <c r="E50" s="38" t="s">
         <v>415</v>
       </c>
-      <c r="F50" s="40" t="s">
+      <c r="F50" s="38" t="s">
         <v>268</v>
       </c>
     </row>
     <row r="51" spans="1:6">
-      <c r="A51" s="39">
+      <c r="A51" s="37">
         <v>50</v>
       </c>
-      <c r="B51" s="40" t="s">
+      <c r="B51" s="38" t="s">
         <v>215</v>
       </c>
-      <c r="C51" s="41">
+      <c r="C51" s="39">
         <v>8321</v>
       </c>
-      <c r="D51" s="40" t="s">
+      <c r="D51" s="38" t="s">
         <v>416</v>
       </c>
-      <c r="E51" s="40" t="s">
+      <c r="E51" s="38" t="s">
         <v>417</v>
       </c>
-      <c r="F51" s="40" t="s">
+      <c r="F51" s="38" t="s">
         <v>418</v>
       </c>
     </row>
     <row r="52" spans="1:6">
-      <c r="A52" s="39">
+      <c r="A52" s="37">
         <v>51</v>
       </c>
-      <c r="B52" s="40" t="s">
+      <c r="B52" s="38" t="s">
         <v>216</v>
       </c>
-      <c r="C52" s="41">
+      <c r="C52" s="39">
         <v>2151</v>
       </c>
-      <c r="D52" s="40" t="s">
+      <c r="D52" s="38" t="s">
         <v>265</v>
       </c>
-      <c r="E52" s="40" t="s">
+      <c r="E52" s="38" t="s">
         <v>419</v>
       </c>
-      <c r="F52" s="40" t="s">
+      <c r="F52" s="38" t="s">
         <v>266</v>
       </c>
     </row>
     <row r="53" spans="1:6">
-      <c r="A53" s="39">
+      <c r="A53" s="37">
         <v>52</v>
       </c>
-      <c r="B53" s="40" t="s">
+      <c r="B53" s="38" t="s">
         <v>217</v>
       </c>
-      <c r="C53" s="41">
+      <c r="C53" s="39">
         <v>3115</v>
       </c>
-      <c r="D53" s="40" t="s">
+      <c r="D53" s="38" t="s">
         <v>335</v>
       </c>
-      <c r="E53" s="40" t="s">
+      <c r="E53" s="38" t="s">
         <v>420</v>
       </c>
-      <c r="F53" s="40" t="s">
+      <c r="F53" s="38" t="s">
         <v>421</v>
       </c>
     </row>
     <row r="54" spans="1:6">
-      <c r="A54" s="39">
+      <c r="A54" s="37">
         <v>53</v>
       </c>
-      <c r="B54" s="40" t="s">
+      <c r="B54" s="38" t="s">
         <v>218</v>
       </c>
-      <c r="C54" s="41">
+      <c r="C54" s="39">
         <v>2431</v>
       </c>
-      <c r="D54" s="40" t="s">
+      <c r="D54" s="38" t="s">
         <v>422</v>
       </c>
-      <c r="E54" s="40" t="s">
+      <c r="E54" s="38" t="s">
         <v>423</v>
       </c>
-      <c r="F54" s="40" t="s">
+      <c r="F54" s="38" t="s">
         <v>424</v>
       </c>
     </row>
     <row r="55" spans="1:6">
-      <c r="A55" s="39">
+      <c r="A55" s="37">
         <v>54</v>
       </c>
-      <c r="B55" s="40" t="s">
+      <c r="B55" s="38" t="s">
         <v>219</v>
       </c>
-      <c r="C55" s="41">
+      <c r="C55" s="39">
         <v>3118</v>
       </c>
-      <c r="D55" s="40" t="s">
+      <c r="D55" s="38" t="s">
         <v>288</v>
       </c>
-      <c r="E55" s="40" t="s">
+      <c r="E55" s="38" t="s">
         <v>425</v>
       </c>
-      <c r="F55" s="40" t="s">
+      <c r="F55" s="38" t="s">
         <v>304</v>
       </c>
     </row>
-    <row r="56" spans="1:6" s="45" customFormat="1">
-      <c r="A56" s="42">
+    <row r="56" spans="1:6" s="43" customFormat="1">
+      <c r="A56" s="40">
         <v>55</v>
       </c>
-      <c r="B56" s="43" t="s">
+      <c r="B56" s="41" t="s">
         <v>220</v>
       </c>
-      <c r="C56" s="44">
+      <c r="C56" s="42">
         <v>2166</v>
       </c>
-      <c r="D56" s="43" t="s">
+      <c r="D56" s="41" t="s">
         <v>295</v>
       </c>
-      <c r="E56" s="43" t="s">
+      <c r="E56" s="41" t="s">
         <v>426</v>
       </c>
-      <c r="F56" s="43" t="s">
+      <c r="F56" s="41" t="s">
         <v>427</v>
       </c>
     </row>
     <row r="57" spans="1:6">
-      <c r="A57" s="39">
+      <c r="A57" s="37">
         <v>56</v>
       </c>
-      <c r="B57" s="40" t="s">
+      <c r="B57" s="38" t="s">
         <v>221</v>
       </c>
-      <c r="C57" s="41">
+      <c r="C57" s="39">
         <v>4110</v>
       </c>
-      <c r="D57" s="40" t="s">
+      <c r="D57" s="38" t="s">
         <v>428</v>
       </c>
-      <c r="E57" s="40" t="s">
+      <c r="E57" s="38" t="s">
         <v>429</v>
       </c>
-      <c r="F57" s="40" t="s">
+      <c r="F57" s="38" t="s">
         <v>430</v>
       </c>
     </row>
     <row r="58" spans="1:6">
-      <c r="A58" s="39">
+      <c r="A58" s="37">
         <v>57</v>
       </c>
-      <c r="B58" s="40" t="s">
+      <c r="B58" s="38" t="s">
         <v>222</v>
       </c>
-      <c r="C58" s="41" t="s">
+      <c r="C58" s="39" t="s">
         <v>259</v>
       </c>
-      <c r="D58" s="40" t="s">
+      <c r="D58" s="38" t="s">
         <v>431</v>
       </c>
-      <c r="E58" s="40" t="s">
+      <c r="E58" s="38" t="s">
         <v>432</v>
       </c>
-      <c r="F58" s="40" t="s">
+      <c r="F58" s="38" t="s">
         <v>433</v>
       </c>
     </row>
     <row r="59" spans="1:6">
-      <c r="A59" s="39">
+      <c r="A59" s="37">
         <v>58</v>
       </c>
-      <c r="B59" s="40" t="s">
+      <c r="B59" s="38" t="s">
         <v>223</v>
       </c>
-      <c r="C59" s="41">
+      <c r="C59" s="39">
         <v>7422</v>
       </c>
-      <c r="D59" s="40" t="s">
+      <c r="D59" s="38" t="s">
         <v>434</v>
       </c>
-      <c r="E59" s="40" t="s">
+      <c r="E59" s="38" t="s">
         <v>435</v>
       </c>
-      <c r="F59" s="40" t="s">
+      <c r="F59" s="38" t="s">
         <v>436</v>
       </c>
     </row>
     <row r="60" spans="1:6">
-      <c r="A60" s="39">
+      <c r="A60" s="37">
         <v>59</v>
       </c>
-      <c r="B60" s="40" t="s">
+      <c r="B60" s="38" t="s">
         <v>224</v>
       </c>
-      <c r="C60" s="41">
+      <c r="C60" s="39">
         <v>3512</v>
       </c>
-      <c r="D60" s="40" t="s">
+      <c r="D60" s="38" t="s">
         <v>437</v>
       </c>
-      <c r="E60" s="40" t="s">
+      <c r="E60" s="38" t="s">
         <v>296</v>
       </c>
-      <c r="F60" s="40" t="s">
+      <c r="F60" s="38" t="s">
         <v>438</v>
       </c>
     </row>
     <row r="61" spans="1:6">
-      <c r="A61" s="39">
+      <c r="A61" s="37">
         <v>60</v>
       </c>
-      <c r="B61" s="40" t="s">
+      <c r="B61" s="38" t="s">
         <v>226</v>
       </c>
-      <c r="C61" s="41">
+      <c r="C61" s="39">
         <v>7422</v>
       </c>
-      <c r="D61" s="40" t="s">
+      <c r="D61" s="38" t="s">
         <v>293</v>
       </c>
-      <c r="E61" s="40" t="s">
+      <c r="E61" s="38" t="s">
         <v>439</v>
       </c>
-      <c r="F61" s="40" t="s">
+      <c r="F61" s="38" t="s">
         <v>440</v>
       </c>
     </row>
-    <row r="62" spans="1:6" s="45" customFormat="1">
-      <c r="A62" s="42">
+    <row r="62" spans="1:6" s="43" customFormat="1">
+      <c r="A62" s="40">
         <v>61</v>
       </c>
-      <c r="B62" s="43" t="s">
+      <c r="B62" s="41" t="s">
         <v>227</v>
       </c>
-      <c r="C62" s="44">
+      <c r="C62" s="42">
         <v>3119</v>
       </c>
-      <c r="D62" s="43" t="s">
+      <c r="D62" s="41" t="s">
         <v>267</v>
       </c>
-      <c r="E62" s="43" t="s">
+      <c r="E62" s="41" t="s">
         <v>441</v>
       </c>
-      <c r="F62" s="43" t="s">
+      <c r="F62" s="41" t="s">
         <v>292</v>
       </c>
     </row>
-    <row r="63" spans="1:6" s="45" customFormat="1">
-      <c r="A63" s="42">
+    <row r="63" spans="1:6" s="43" customFormat="1">
+      <c r="A63" s="40">
         <v>62</v>
       </c>
-      <c r="B63" s="43" t="s">
+      <c r="B63" s="41" t="s">
         <v>228</v>
       </c>
-      <c r="C63" s="44">
+      <c r="C63" s="42">
         <v>7422</v>
       </c>
-      <c r="D63" s="43" t="s">
+      <c r="D63" s="41" t="s">
         <v>177</v>
       </c>
-      <c r="E63" s="43" t="s">
+      <c r="E63" s="41" t="s">
         <v>442</v>
       </c>
-      <c r="F63" s="43" t="s">
+      <c r="F63" s="41" t="s">
         <v>443</v>
       </c>
     </row>
     <row r="64" spans="1:6">
-      <c r="A64" s="39">
+      <c r="A64" s="37">
         <v>63</v>
       </c>
-      <c r="B64" s="40" t="s">
+      <c r="B64" s="38" t="s">
         <v>229</v>
       </c>
-      <c r="C64" s="41">
+      <c r="C64" s="39">
         <v>2166</v>
       </c>
-      <c r="D64" s="40" t="s">
+      <c r="D64" s="38" t="s">
         <v>295</v>
       </c>
-      <c r="E64" s="40" t="s">
+      <c r="E64" s="38" t="s">
         <v>444</v>
       </c>
-      <c r="F64" s="40" t="s">
+      <c r="F64" s="38" t="s">
         <v>445</v>
       </c>
     </row>
     <row r="65" spans="1:6">
-      <c r="A65" s="39">
+      <c r="A65" s="37">
         <v>64</v>
       </c>
-      <c r="B65" s="40" t="s">
+      <c r="B65" s="38" t="s">
         <v>143</v>
       </c>
-      <c r="C65" s="41">
+      <c r="C65" s="39">
         <v>3322</v>
       </c>
-      <c r="D65" s="40" t="s">
+      <c r="D65" s="38" t="s">
         <v>281</v>
       </c>
-      <c r="E65" s="40" t="s">
+      <c r="E65" s="38" t="s">
         <v>446</v>
       </c>
-      <c r="F65" s="40" t="s">
+      <c r="F65" s="38" t="s">
         <v>447</v>
       </c>
     </row>
     <row r="66" spans="1:6">
-      <c r="A66" s="39">
+      <c r="A66" s="37">
         <v>65</v>
       </c>
-      <c r="B66" s="40" t="s">
+      <c r="B66" s="38" t="s">
         <v>230</v>
       </c>
-      <c r="C66" s="41">
+      <c r="C66" s="39">
         <v>7411</v>
       </c>
-      <c r="D66" s="40" t="s">
+      <c r="D66" s="38" t="s">
         <v>263</v>
       </c>
-      <c r="E66" s="40" t="s">
+      <c r="E66" s="38" t="s">
         <v>448</v>
       </c>
-      <c r="F66" s="40" t="s">
+      <c r="F66" s="38" t="s">
         <v>305</v>
       </c>
     </row>
     <row r="67" spans="1:6">
-      <c r="A67" s="39">
+      <c r="A67" s="37">
         <v>66</v>
       </c>
-      <c r="B67" s="40" t="s">
+      <c r="B67" s="38" t="s">
         <v>231</v>
       </c>
-      <c r="C67" s="41">
+      <c r="C67" s="39">
         <v>8131</v>
       </c>
-      <c r="D67" s="40" t="s">
+      <c r="D67" s="38" t="s">
         <v>130</v>
       </c>
-      <c r="E67" s="40" t="s">
+      <c r="E67" s="38" t="s">
         <v>449</v>
       </c>
-      <c r="F67" s="40" t="s">
+      <c r="F67" s="38" t="s">
         <v>450</v>
       </c>
     </row>
     <row r="68" spans="1:6">
-      <c r="A68" s="39">
+      <c r="A68" s="37">
         <v>67</v>
       </c>
-      <c r="B68" s="40" t="s">
+      <c r="B68" s="38" t="s">
         <v>234</v>
       </c>
-      <c r="C68" s="41">
+      <c r="C68" s="39">
         <v>1324</v>
       </c>
-      <c r="D68" s="40" t="s">
+      <c r="D68" s="38" t="s">
         <v>451</v>
       </c>
-      <c r="E68" s="40" t="s">
+      <c r="E68" s="38" t="s">
         <v>452</v>
       </c>
-      <c r="F68" s="40" t="s">
+      <c r="F68" s="38" t="s">
         <v>453</v>
       </c>
     </row>
     <row r="69" spans="1:6">
-      <c r="A69" s="39">
+      <c r="A69" s="37">
         <v>68</v>
       </c>
-      <c r="B69" s="40" t="s">
+      <c r="B69" s="38" t="s">
         <v>235</v>
       </c>
-      <c r="C69" s="41">
+      <c r="C69" s="39">
         <v>7411</v>
       </c>
-      <c r="D69" s="40" t="s">
+      <c r="D69" s="38" t="s">
         <v>263</v>
       </c>
-      <c r="E69" s="40" t="s">
+      <c r="E69" s="38" t="s">
         <v>454</v>
       </c>
-      <c r="F69" s="40" t="s">
+      <c r="F69" s="38" t="s">
         <v>455</v>
       </c>
     </row>
     <row r="70" spans="1:6">
-      <c r="A70" s="39">
+      <c r="A70" s="37">
         <v>69</v>
       </c>
-      <c r="B70" s="40" t="s">
+      <c r="B70" s="38" t="s">
         <v>236</v>
       </c>
-      <c r="C70" s="41">
+      <c r="C70" s="39">
         <v>2166</v>
       </c>
-      <c r="D70" s="40" t="s">
+      <c r="D70" s="38" t="s">
         <v>456</v>
       </c>
-      <c r="E70" s="40" t="s">
+      <c r="E70" s="38" t="s">
         <v>291</v>
       </c>
-      <c r="F70" s="40" t="s">
+      <c r="F70" s="38" t="s">
         <v>457</v>
       </c>
     </row>
     <row r="71" spans="1:6">
-      <c r="A71" s="39">
+      <c r="A71" s="37">
         <v>70</v>
       </c>
-      <c r="B71" s="40" t="s">
+      <c r="B71" s="38" t="s">
         <v>237</v>
       </c>
-      <c r="C71" s="41">
+      <c r="C71" s="39">
         <v>3315</v>
       </c>
-      <c r="D71" s="40" t="s">
+      <c r="D71" s="38" t="s">
         <v>290</v>
       </c>
-      <c r="E71" s="40" t="s">
+      <c r="E71" s="38" t="s">
         <v>458</v>
       </c>
-      <c r="F71" s="40" t="s">
+      <c r="F71" s="38" t="s">
         <v>459</v>
       </c>
     </row>
     <row r="72" spans="1:6">
-      <c r="A72" s="39">
+      <c r="A72" s="37">
         <v>71</v>
       </c>
-      <c r="B72" s="40" t="s">
+      <c r="B72" s="38" t="s">
         <v>238</v>
       </c>
-      <c r="C72" s="41">
+      <c r="C72" s="39">
         <v>2143</v>
       </c>
-      <c r="D72" s="40" t="s">
+      <c r="D72" s="38" t="s">
         <v>460</v>
       </c>
-      <c r="E72" s="40" t="s">
+      <c r="E72" s="38" t="s">
         <v>461</v>
       </c>
-      <c r="F72" s="40" t="s">
+      <c r="F72" s="38" t="s">
         <v>462</v>
       </c>
     </row>
     <row r="73" spans="1:6">
-      <c r="A73" s="39">
+      <c r="A73" s="37">
         <v>72</v>
       </c>
-      <c r="B73" s="40" t="s">
+      <c r="B73" s="38" t="s">
         <v>239</v>
       </c>
-      <c r="C73" s="41">
+      <c r="C73" s="39">
         <v>3118</v>
       </c>
-      <c r="D73" s="40" t="s">
+      <c r="D73" s="38" t="s">
         <v>289</v>
       </c>
-      <c r="E73" s="40" t="s">
+      <c r="E73" s="38" t="s">
         <v>463</v>
       </c>
-      <c r="F73" s="40" t="s">
+      <c r="F73" s="38" t="s">
         <v>464</v>
       </c>
     </row>
     <row r="74" spans="1:6">
-      <c r="A74" s="39">
+      <c r="A74" s="37">
         <v>73</v>
       </c>
-      <c r="B74" s="40" t="s">
+      <c r="B74" s="38" t="s">
         <v>240</v>
       </c>
-      <c r="C74" s="41">
+      <c r="C74" s="39">
         <v>1323</v>
       </c>
-      <c r="D74" s="40" t="s">
+      <c r="D74" s="38" t="s">
         <v>465</v>
       </c>
-      <c r="E74" s="40" t="s">
+      <c r="E74" s="38" t="s">
         <v>466</v>
       </c>
-      <c r="F74" s="40" t="s">
+      <c r="F74" s="38" t="s">
         <v>467</v>
       </c>
     </row>
     <row r="75" spans="1:6">
-      <c r="A75" s="39">
+      <c r="A75" s="37">
         <v>74</v>
       </c>
-      <c r="B75" s="40" t="s">
+      <c r="B75" s="38" t="s">
         <v>241</v>
       </c>
-      <c r="C75" s="41">
+      <c r="C75" s="39">
         <v>3322</v>
       </c>
-      <c r="D75" s="40" t="s">
+      <c r="D75" s="38" t="s">
         <v>256</v>
       </c>
-      <c r="E75" s="40" t="s">
+      <c r="E75" s="38" t="s">
         <v>468</v>
       </c>
-      <c r="F75" s="40" t="s">
+      <c r="F75" s="38" t="s">
         <v>424</v>
       </c>
     </row>
     <row r="76" spans="1:6">
-      <c r="A76" s="39">
+      <c r="A76" s="37">
         <v>75</v>
       </c>
-      <c r="B76" s="40" t="s">
+      <c r="B76" s="38" t="s">
         <v>242</v>
       </c>
-      <c r="C76" s="41">
+      <c r="C76" s="39">
         <v>5223</v>
       </c>
-      <c r="D76" s="40" t="s">
+      <c r="D76" s="38" t="s">
         <v>307</v>
       </c>
-      <c r="E76" s="40" t="s">
+      <c r="E76" s="38" t="s">
         <v>308</v>
       </c>
-      <c r="F76" s="40" t="s">
+      <c r="F76" s="38" t="s">
         <v>469</v>
       </c>
     </row>
     <row r="77" spans="1:6">
-      <c r="A77" s="39">
+      <c r="A77" s="37">
         <v>76</v>
       </c>
-      <c r="B77" s="40" t="s">
+      <c r="B77" s="38" t="s">
         <v>243</v>
       </c>
-      <c r="C77" s="41" t="s">
+      <c r="C77" s="39" t="s">
         <v>270</v>
       </c>
-      <c r="D77" s="40" t="s">
+      <c r="D77" s="38" t="s">
         <v>243</v>
       </c>
-      <c r="E77" s="40" t="s">
+      <c r="E77" s="38" t="s">
         <v>470</v>
       </c>
-      <c r="F77" s="40" t="s">
+      <c r="F77" s="38" t="s">
         <v>471</v>
       </c>
     </row>
     <row r="78" spans="1:6">
-      <c r="A78" s="39">
+      <c r="A78" s="37">
         <v>77</v>
       </c>
-      <c r="B78" s="40" t="s">
+      <c r="B78" s="38" t="s">
         <v>244</v>
       </c>
-      <c r="C78" s="41">
+      <c r="C78" s="39">
         <v>1420</v>
       </c>
-      <c r="D78" s="40" t="s">
+      <c r="D78" s="38" t="s">
         <v>472</v>
       </c>
-      <c r="E78" s="40" t="s">
+      <c r="E78" s="38" t="s">
         <v>473</v>
       </c>
-      <c r="F78" s="40" t="s">
+      <c r="F78" s="38" t="s">
         <v>474</v>
       </c>
     </row>
     <row r="79" spans="1:6">
-      <c r="A79" s="39">
+      <c r="A79" s="37">
         <v>78</v>
       </c>
-      <c r="B79" s="40" t="s">
+      <c r="B79" s="38" t="s">
         <v>475</v>
       </c>
-      <c r="C79" s="41">
+      <c r="C79" s="39">
         <v>3315</v>
       </c>
-      <c r="D79" s="40" t="s">
+      <c r="D79" s="38" t="s">
         <v>476</v>
       </c>
-      <c r="E79" s="40" t="s">
+      <c r="E79" s="38" t="s">
         <v>477</v>
       </c>
-      <c r="F79" s="40" t="s">
+      <c r="F79" s="38" t="s">
         <v>478</v>
       </c>
     </row>
     <row r="80" spans="1:6">
-      <c r="A80" s="39">
+      <c r="A80" s="37">
         <v>79</v>
       </c>
-      <c r="B80" s="40" t="s">
+      <c r="B80" s="38" t="s">
         <v>246</v>
       </c>
-      <c r="C80" s="41">
+      <c r="C80" s="39">
         <v>3322</v>
       </c>
-      <c r="D80" s="40" t="s">
+      <c r="D80" s="38" t="s">
         <v>479</v>
       </c>
-      <c r="E80" s="40" t="s">
+      <c r="E80" s="38" t="s">
         <v>480</v>
       </c>
-      <c r="F80" s="40" t="s">
+      <c r="F80" s="38" t="s">
         <v>481</v>
       </c>
     </row>
     <row r="81" spans="1:6">
-      <c r="A81" s="39">
+      <c r="A81" s="37">
         <v>80</v>
       </c>
-      <c r="B81" s="40" t="s">
+      <c r="B81" s="38" t="s">
         <v>297</v>
       </c>
-      <c r="C81" s="41">
+      <c r="C81" s="39">
         <v>7222</v>
       </c>
-      <c r="D81" s="40" t="s">
+      <c r="D81" s="38" t="s">
         <v>482</v>
       </c>
-      <c r="E81" s="40" t="s">
+      <c r="E81" s="38" t="s">
         <v>483</v>
       </c>
-      <c r="F81" s="40" t="s">
+      <c r="F81" s="38" t="s">
         <v>484</v>
       </c>
     </row>
     <row r="82" spans="1:6">
-      <c r="A82" s="39">
+      <c r="A82" s="37">
         <v>81</v>
       </c>
-      <c r="B82" s="40" t="s">
+      <c r="B82" s="38" t="s">
         <v>298</v>
       </c>
-      <c r="C82" s="41">
+      <c r="C82" s="39">
         <v>3139</v>
       </c>
-      <c r="D82" s="40" t="s">
+      <c r="D82" s="38" t="s">
         <v>299</v>
       </c>
-      <c r="E82" s="40" t="s">
+      <c r="E82" s="38" t="s">
         <v>485</v>
       </c>
-      <c r="F82" s="40" t="s">
+      <c r="F82" s="38" t="s">
         <v>300</v>
       </c>
     </row>
     <row r="83" spans="1:6">
-      <c r="A83" s="39">
+      <c r="A83" s="37">
         <v>82</v>
       </c>
-      <c r="B83" s="40" t="s">
+      <c r="B83" s="38" t="s">
         <v>272</v>
       </c>
-      <c r="C83" s="41">
+      <c r="C83" s="39">
         <v>7223</v>
       </c>
-      <c r="D83" s="40" t="s">
+      <c r="D83" s="38" t="s">
         <v>273</v>
       </c>
-      <c r="E83" s="40" t="s">
+      <c r="E83" s="38" t="s">
         <v>486</v>
       </c>
-      <c r="F83" s="40" t="s">
+      <c r="F83" s="38" t="s">
         <v>487</v>
       </c>
     </row>
-    <row r="84" spans="1:6">
-      <c r="A84" s="39">
+    <row r="84" spans="1:6" ht="15.75" thickBot="1">
+      <c r="A84" s="37">
         <v>83</v>
       </c>
-      <c r="B84" s="40" t="s">
+      <c r="B84" s="38" t="s">
         <v>250</v>
       </c>
-      <c r="C84" s="41">
+      <c r="C84" s="39">
         <v>7222</v>
       </c>
-      <c r="D84" s="40" t="s">
+      <c r="D84" s="38" t="s">
         <v>301</v>
       </c>
-      <c r="E84" s="40" t="s">
+      <c r="E84" s="38" t="s">
         <v>302</v>
       </c>
-      <c r="F84" s="40" t="s">
+      <c r="F84" s="38" t="s">
         <v>303</v>
       </c>
     </row>
-    <row r="85" spans="1:6">
-      <c r="B85" s="34"/>
-      <c r="C85" s="35"/>
-      <c r="D85" s="34"/>
-      <c r="E85" s="34"/>
-      <c r="F85" s="34"/>
-    </row>
-    <row r="86" spans="1:6">
-      <c r="B86" s="34"/>
-      <c r="C86" s="35"/>
-      <c r="D86" s="34"/>
-      <c r="E86" s="34"/>
-      <c r="F86" s="34"/>
-    </row>
-    <row r="87" spans="1:6">
-      <c r="B87" s="34"/>
-      <c r="C87" s="35"/>
-      <c r="D87" s="34"/>
-      <c r="E87" s="34"/>
-      <c r="F87" s="34"/>
-    </row>
-    <row r="88" spans="1:6">
-      <c r="B88" s="34"/>
-      <c r="C88" s="35"/>
-      <c r="D88" s="34"/>
-      <c r="E88" s="34"/>
-      <c r="F88" s="34"/>
-    </row>
-    <row r="89" spans="1:6">
-      <c r="B89" s="34"/>
-      <c r="C89" s="35"/>
-      <c r="D89" s="34"/>
-      <c r="E89" s="34"/>
-      <c r="F89" s="34"/>
+    <row r="85" spans="1:6" ht="90.75" thickBot="1">
+      <c r="A85" s="60">
+        <v>84</v>
+      </c>
+      <c r="B85" s="61" t="s">
+        <v>489</v>
+      </c>
+      <c r="C85" s="62" t="s">
+        <v>490</v>
+      </c>
+      <c r="D85" s="61" t="s">
+        <v>491</v>
+      </c>
+      <c r="E85" s="61" t="s">
+        <v>492</v>
+      </c>
+      <c r="F85" s="61" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" ht="180.75" thickBot="1">
+      <c r="A86" s="63">
+        <v>85</v>
+      </c>
+      <c r="B86" s="64" t="s">
+        <v>493</v>
+      </c>
+      <c r="C86" s="64"/>
+      <c r="D86" s="64" t="s">
+        <v>494</v>
+      </c>
+      <c r="E86" s="64" t="s">
+        <v>495</v>
+      </c>
+      <c r="F86" s="64"/>
+    </row>
+    <row r="87" spans="1:6" ht="90.75" thickBot="1">
+      <c r="A87" s="63">
+        <v>86</v>
+      </c>
+      <c r="B87" s="64" t="s">
+        <v>496</v>
+      </c>
+      <c r="C87" s="64"/>
+      <c r="D87" s="64" t="s">
+        <v>497</v>
+      </c>
+      <c r="E87" s="64" t="s">
+        <v>498</v>
+      </c>
+      <c r="F87" s="64"/>
+    </row>
+    <row r="88" spans="1:6" ht="150.75" thickBot="1">
+      <c r="A88" s="63">
+        <v>87</v>
+      </c>
+      <c r="B88" s="64" t="s">
+        <v>499</v>
+      </c>
+      <c r="C88" s="64"/>
+      <c r="D88" s="64" t="s">
+        <v>189</v>
+      </c>
+      <c r="E88" s="64" t="s">
+        <v>500</v>
+      </c>
+      <c r="F88" s="64"/>
+    </row>
+    <row r="89" spans="1:6" ht="135.75" thickBot="1">
+      <c r="A89" s="63">
+        <v>88</v>
+      </c>
+      <c r="B89" s="64" t="s">
+        <v>501</v>
+      </c>
+      <c r="C89" s="64"/>
+      <c r="D89" s="64" t="s">
+        <v>179</v>
+      </c>
+      <c r="E89" s="64" t="s">
+        <v>502</v>
+      </c>
+      <c r="F89" s="64"/>
+    </row>
+    <row r="90" spans="1:6" ht="105.75" thickBot="1">
+      <c r="A90" s="63">
+        <v>89</v>
+      </c>
+      <c r="B90" s="64" t="s">
+        <v>503</v>
+      </c>
+      <c r="C90" s="64"/>
+      <c r="D90" s="64" t="s">
+        <v>504</v>
+      </c>
+      <c r="E90" s="64" t="s">
+        <v>505</v>
+      </c>
+      <c r="F90" s="65"/>
+    </row>
+    <row r="91" spans="1:6" ht="165.75" thickBot="1">
+      <c r="A91" s="63">
+        <v>90</v>
+      </c>
+      <c r="B91" s="64" t="s">
+        <v>506</v>
+      </c>
+      <c r="C91" s="64"/>
+      <c r="D91" s="64" t="s">
+        <v>119</v>
+      </c>
+      <c r="E91" s="64" t="s">
+        <v>507</v>
+      </c>
+      <c r="F91" s="65"/>
+    </row>
+    <row r="92" spans="1:6" ht="120.75" thickBot="1">
+      <c r="A92" s="63">
+        <v>91</v>
+      </c>
+      <c r="B92" s="64" t="s">
+        <v>508</v>
+      </c>
+      <c r="C92" s="64"/>
+      <c r="D92" s="64" t="s">
+        <v>138</v>
+      </c>
+      <c r="E92" s="64" t="s">
+        <v>509</v>
+      </c>
+      <c r="F92" s="65"/>
+    </row>
+    <row r="93" spans="1:6" ht="165.75" thickBot="1">
+      <c r="A93" s="63">
+        <v>92</v>
+      </c>
+      <c r="B93" s="64" t="s">
+        <v>510</v>
+      </c>
+      <c r="C93" s="64"/>
+      <c r="D93" s="64" t="s">
+        <v>511</v>
+      </c>
+      <c r="E93" s="65" t="s">
+        <v>512</v>
+      </c>
+      <c r="F93" s="65"/>
+    </row>
+    <row r="94" spans="1:6" ht="210.75" thickBot="1">
+      <c r="A94" s="63">
+        <v>93</v>
+      </c>
+      <c r="B94" s="64" t="s">
+        <v>513</v>
+      </c>
+      <c r="C94" s="64"/>
+      <c r="D94" s="64" t="s">
+        <v>280</v>
+      </c>
+      <c r="E94" s="64" t="s">
+        <v>514</v>
+      </c>
+      <c r="F94" s="65"/>
+    </row>
+    <row r="95" spans="1:6" ht="165.75" thickBot="1">
+      <c r="A95" s="63">
+        <v>94</v>
+      </c>
+      <c r="B95" s="64" t="s">
+        <v>515</v>
+      </c>
+      <c r="C95" s="64"/>
+      <c r="D95" s="64" t="s">
+        <v>516</v>
+      </c>
+      <c r="E95" s="64" t="s">
+        <v>517</v>
+      </c>
+      <c r="F95" s="65"/>
+    </row>
+    <row r="96" spans="1:6" ht="120.75" thickBot="1">
+      <c r="A96" s="63">
+        <v>95</v>
+      </c>
+      <c r="B96" s="64" t="s">
+        <v>518</v>
+      </c>
+      <c r="C96" s="64"/>
+      <c r="D96" s="64" t="s">
+        <v>126</v>
+      </c>
+      <c r="E96" s="64" t="s">
+        <v>519</v>
+      </c>
+      <c r="F96" s="65"/>
+    </row>
+    <row r="97" spans="1:6" ht="150.75" thickBot="1">
+      <c r="A97" s="63">
+        <v>96</v>
+      </c>
+      <c r="B97" s="64" t="s">
+        <v>520</v>
+      </c>
+      <c r="C97" s="64"/>
+      <c r="D97" s="64" t="s">
+        <v>123</v>
+      </c>
+      <c r="E97" s="65" t="s">
+        <v>521</v>
+      </c>
+      <c r="F97" s="65"/>
+    </row>
+    <row r="98" spans="1:6" ht="90.75" thickBot="1">
+      <c r="A98" s="63">
+        <v>97</v>
+      </c>
+      <c r="B98" s="64" t="s">
+        <v>522</v>
+      </c>
+      <c r="C98" s="64"/>
+      <c r="D98" s="64" t="s">
+        <v>69</v>
+      </c>
+      <c r="E98" s="64" t="s">
+        <v>523</v>
+      </c>
+      <c r="F98" s="65"/>
+    </row>
+    <row r="99" spans="1:6" ht="135.75" thickBot="1">
+      <c r="A99" s="63">
+        <v>98</v>
+      </c>
+      <c r="B99" s="64" t="s">
+        <v>524</v>
+      </c>
+      <c r="C99" s="64"/>
+      <c r="D99" s="64" t="s">
+        <v>525</v>
+      </c>
+      <c r="E99" s="64" t="s">
+        <v>526</v>
+      </c>
+      <c r="F99" s="65"/>
+    </row>
+    <row r="100" spans="1:6" ht="105.75" thickBot="1">
+      <c r="A100" s="63">
+        <v>99</v>
+      </c>
+      <c r="B100" s="64" t="s">
+        <v>527</v>
+      </c>
+      <c r="C100" s="64"/>
+      <c r="D100" s="64" t="s">
+        <v>528</v>
+      </c>
+      <c r="E100" s="65" t="s">
+        <v>529</v>
+      </c>
+      <c r="F100" s="65"/>
+    </row>
+    <row r="101" spans="1:6" ht="210.75" thickBot="1">
+      <c r="A101" s="63">
+        <v>100</v>
+      </c>
+      <c r="B101" s="64" t="s">
+        <v>530</v>
+      </c>
+      <c r="C101" s="64"/>
+      <c r="D101" s="64" t="s">
+        <v>531</v>
+      </c>
+      <c r="E101" s="64" t="s">
+        <v>532</v>
+      </c>
+      <c r="F101" s="65"/>
+    </row>
+    <row r="102" spans="1:6" ht="180.75" thickBot="1">
+      <c r="A102" s="63">
+        <v>101</v>
+      </c>
+      <c r="B102" s="64" t="s">
+        <v>533</v>
+      </c>
+      <c r="C102" s="64"/>
+      <c r="D102" s="64" t="s">
+        <v>69</v>
+      </c>
+      <c r="E102" s="64" t="s">
+        <v>534</v>
+      </c>
+      <c r="F102" s="65"/>
+    </row>
+    <row r="103" spans="1:6" ht="135.75" thickBot="1">
+      <c r="A103" s="63">
+        <v>102</v>
+      </c>
+      <c r="B103" s="64" t="s">
+        <v>535</v>
+      </c>
+      <c r="C103" s="64"/>
+      <c r="D103" s="64" t="s">
+        <v>536</v>
+      </c>
+      <c r="E103" s="64" t="s">
+        <v>537</v>
+      </c>
+      <c r="F103" s="65"/>
+    </row>
+    <row r="104" spans="1:6" ht="135.75" thickBot="1">
+      <c r="A104" s="63">
+        <v>103</v>
+      </c>
+      <c r="B104" s="64" t="s">
+        <v>538</v>
+      </c>
+      <c r="C104" s="64"/>
+      <c r="D104" s="64" t="s">
+        <v>68</v>
+      </c>
+      <c r="E104" s="65" t="s">
+        <v>539</v>
+      </c>
+      <c r="F104" s="65"/>
+    </row>
+    <row r="105" spans="1:6" ht="120.75" thickBot="1">
+      <c r="A105" s="63">
+        <v>104</v>
+      </c>
+      <c r="B105" s="64" t="s">
+        <v>540</v>
+      </c>
+      <c r="C105" s="64"/>
+      <c r="D105" s="64" t="s">
+        <v>541</v>
+      </c>
+      <c r="E105" s="64" t="s">
+        <v>542</v>
+      </c>
+      <c r="F105" s="65"/>
+    </row>
+    <row r="106" spans="1:6" ht="165.75" thickBot="1">
+      <c r="A106" s="63">
+        <v>105</v>
+      </c>
+      <c r="B106" s="64" t="s">
+        <v>543</v>
+      </c>
+      <c r="C106" s="64"/>
+      <c r="D106" s="64" t="s">
+        <v>544</v>
+      </c>
+      <c r="E106" s="65" t="s">
+        <v>545</v>
+      </c>
+      <c r="F106" s="65"/>
+    </row>
+    <row r="107" spans="1:6" ht="195.75" thickBot="1">
+      <c r="A107" s="63">
+        <v>106</v>
+      </c>
+      <c r="B107" s="64" t="s">
+        <v>546</v>
+      </c>
+      <c r="C107" s="64"/>
+      <c r="D107" s="64" t="s">
+        <v>94</v>
+      </c>
+      <c r="E107" s="64" t="s">
+        <v>547</v>
+      </c>
+      <c r="F107" s="65"/>
+    </row>
+    <row r="108" spans="1:6" ht="75.75" thickBot="1">
+      <c r="A108" s="63">
+        <v>107</v>
+      </c>
+      <c r="B108" s="64" t="s">
+        <v>548</v>
+      </c>
+      <c r="C108" s="64"/>
+      <c r="D108" s="64" t="s">
+        <v>54</v>
+      </c>
+      <c r="E108" s="65" t="s">
+        <v>549</v>
+      </c>
+      <c r="F108" s="65"/>
+    </row>
+    <row r="109" spans="1:6" ht="120.75" thickBot="1">
+      <c r="A109" s="63">
+        <v>108</v>
+      </c>
+      <c r="B109" s="64" t="s">
+        <v>550</v>
+      </c>
+      <c r="C109" s="64"/>
+      <c r="D109" s="64" t="s">
+        <v>551</v>
+      </c>
+      <c r="E109" s="64" t="s">
+        <v>552</v>
+      </c>
+      <c r="F109" s="65"/>
+    </row>
+    <row r="110" spans="1:6" ht="135.75" thickBot="1">
+      <c r="A110" s="63">
+        <v>109</v>
+      </c>
+      <c r="B110" s="64" t="s">
+        <v>553</v>
+      </c>
+      <c r="C110" s="64"/>
+      <c r="D110" s="64" t="s">
+        <v>177</v>
+      </c>
+      <c r="E110" s="65" t="s">
+        <v>554</v>
+      </c>
+      <c r="F110" s="65"/>
+    </row>
+    <row r="111" spans="1:6" ht="150.75" thickBot="1">
+      <c r="A111" s="63">
+        <v>110</v>
+      </c>
+      <c r="B111" s="64" t="s">
+        <v>555</v>
+      </c>
+      <c r="C111" s="64"/>
+      <c r="D111" s="64" t="s">
+        <v>159</v>
+      </c>
+      <c r="E111" s="64" t="s">
+        <v>556</v>
+      </c>
+      <c r="F111" s="65"/>
+    </row>
+    <row r="112" spans="1:6" ht="135.75" thickBot="1">
+      <c r="A112" s="63">
+        <v>111</v>
+      </c>
+      <c r="B112" s="64" t="s">
+        <v>557</v>
+      </c>
+      <c r="C112" s="64"/>
+      <c r="D112" s="64" t="s">
+        <v>168</v>
+      </c>
+      <c r="E112" s="64" t="s">
+        <v>558</v>
+      </c>
+      <c r="F112" s="65"/>
+    </row>
+    <row r="113" spans="1:6" ht="120.75" thickBot="1">
+      <c r="A113" s="63">
+        <v>112</v>
+      </c>
+      <c r="B113" s="64" t="s">
+        <v>559</v>
+      </c>
+      <c r="C113" s="64"/>
+      <c r="D113" s="64" t="s">
+        <v>117</v>
+      </c>
+      <c r="E113" s="64" t="s">
+        <v>560</v>
+      </c>
+      <c r="F113" s="65"/>
+    </row>
+    <row r="114" spans="1:6" ht="135.75" thickBot="1">
+      <c r="A114" s="63">
+        <v>113</v>
+      </c>
+      <c r="B114" s="64" t="s">
+        <v>561</v>
+      </c>
+      <c r="C114" s="64"/>
+      <c r="D114" s="64" t="s">
+        <v>400</v>
+      </c>
+      <c r="E114" s="64" t="s">
+        <v>562</v>
+      </c>
+      <c r="F114" s="65"/>
+    </row>
+    <row r="115" spans="1:6" ht="120.75" thickBot="1">
+      <c r="A115" s="63">
+        <v>114</v>
+      </c>
+      <c r="B115" s="64" t="s">
+        <v>563</v>
+      </c>
+      <c r="C115" s="64"/>
+      <c r="D115" s="64" t="s">
+        <v>564</v>
+      </c>
+      <c r="E115" s="64" t="s">
+        <v>565</v>
+      </c>
+      <c r="F115" s="65"/>
+    </row>
+    <row r="116" spans="1:6" ht="120.75" thickBot="1">
+      <c r="A116" s="63">
+        <v>115</v>
+      </c>
+      <c r="B116" s="64" t="s">
+        <v>566</v>
+      </c>
+      <c r="C116" s="64"/>
+      <c r="D116" s="64" t="s">
+        <v>567</v>
+      </c>
+      <c r="E116" s="64" t="s">
+        <v>568</v>
+      </c>
+      <c r="F116" s="65"/>
+    </row>
+    <row r="117" spans="1:6" ht="75.75" thickBot="1">
+      <c r="A117" s="63">
+        <v>116</v>
+      </c>
+      <c r="B117" s="64" t="s">
+        <v>569</v>
+      </c>
+      <c r="C117" s="64"/>
+      <c r="D117" s="64" t="s">
+        <v>352</v>
+      </c>
+      <c r="E117" s="64" t="s">
+        <v>570</v>
+      </c>
+      <c r="F117" s="65"/>
+    </row>
+    <row r="118" spans="1:6" ht="105.75" thickBot="1">
+      <c r="A118" s="63">
+        <v>117</v>
+      </c>
+      <c r="B118" s="64" t="s">
+        <v>571</v>
+      </c>
+      <c r="C118" s="64"/>
+      <c r="D118" s="64" t="s">
+        <v>151</v>
+      </c>
+      <c r="E118" s="64" t="s">
+        <v>572</v>
+      </c>
+      <c r="F118" s="65"/>
+    </row>
+    <row r="119" spans="1:6" ht="75.75" thickBot="1">
+      <c r="A119" s="63">
+        <v>118</v>
+      </c>
+      <c r="B119" s="64" t="s">
+        <v>573</v>
+      </c>
+      <c r="C119" s="64"/>
+      <c r="D119" s="64" t="s">
+        <v>574</v>
+      </c>
+      <c r="E119" s="64" t="s">
+        <v>575</v>
+      </c>
+      <c r="F119" s="65"/>
+    </row>
+    <row r="120" spans="1:6" ht="150.75" thickBot="1">
+      <c r="A120" s="63">
+        <v>119</v>
+      </c>
+      <c r="B120" s="64" t="s">
+        <v>576</v>
+      </c>
+      <c r="C120" s="64"/>
+      <c r="D120" s="64" t="s">
+        <v>577</v>
+      </c>
+      <c r="E120" s="64" t="s">
+        <v>578</v>
+      </c>
+      <c r="F120" s="65"/>
+    </row>
+    <row r="121" spans="1:6" ht="165.75" thickBot="1">
+      <c r="A121" s="63">
+        <v>120</v>
+      </c>
+      <c r="B121" s="64" t="s">
+        <v>579</v>
+      </c>
+      <c r="C121" s="64"/>
+      <c r="D121" s="64" t="s">
+        <v>352</v>
+      </c>
+      <c r="E121" s="64" t="s">
+        <v>580</v>
+      </c>
+      <c r="F121" s="65"/>
+    </row>
+    <row r="122" spans="1:6" ht="180.75" thickBot="1">
+      <c r="A122" s="63">
+        <v>121</v>
+      </c>
+      <c r="B122" s="64" t="s">
+        <v>581</v>
+      </c>
+      <c r="C122" s="64"/>
+      <c r="D122" s="64" t="s">
+        <v>582</v>
+      </c>
+      <c r="E122" s="64" t="s">
+        <v>583</v>
+      </c>
+      <c r="F122" s="65"/>
+    </row>
+    <row r="123" spans="1:6" ht="165.75" thickBot="1">
+      <c r="A123" s="63">
+        <v>122</v>
+      </c>
+      <c r="B123" s="64" t="s">
+        <v>584</v>
+      </c>
+      <c r="C123" s="64"/>
+      <c r="D123" s="64" t="s">
+        <v>585</v>
+      </c>
+      <c r="E123" s="64" t="s">
+        <v>586</v>
+      </c>
+      <c r="F123" s="65"/>
+    </row>
+    <row r="124" spans="1:6" ht="135.75" thickBot="1">
+      <c r="A124" s="63">
+        <v>123</v>
+      </c>
+      <c r="B124" s="64" t="s">
+        <v>587</v>
+      </c>
+      <c r="C124" s="64"/>
+      <c r="D124" s="64" t="s">
+        <v>588</v>
+      </c>
+      <c r="E124" s="64" t="s">
+        <v>589</v>
+      </c>
+      <c r="F124" s="65"/>
+    </row>
+    <row r="125" spans="1:6" ht="120.75" thickBot="1">
+      <c r="A125" s="63">
+        <v>124</v>
+      </c>
+      <c r="B125" s="64" t="s">
+        <v>590</v>
+      </c>
+      <c r="C125" s="64"/>
+      <c r="D125" s="64" t="s">
+        <v>591</v>
+      </c>
+      <c r="E125" s="64" t="s">
+        <v>592</v>
+      </c>
+      <c r="F125" s="65"/>
+    </row>
+    <row r="126" spans="1:6" ht="120.75" thickBot="1">
+      <c r="A126" s="63">
+        <v>125</v>
+      </c>
+      <c r="B126" s="64" t="s">
+        <v>593</v>
+      </c>
+      <c r="C126" s="64"/>
+      <c r="D126" s="64" t="s">
+        <v>594</v>
+      </c>
+      <c r="E126" s="64" t="s">
+        <v>595</v>
+      </c>
+      <c r="F126" s="65"/>
+    </row>
+    <row r="127" spans="1:6" ht="90.75" thickBot="1">
+      <c r="A127" s="63">
+        <v>126</v>
+      </c>
+      <c r="B127" s="64" t="s">
+        <v>596</v>
+      </c>
+      <c r="C127" s="64"/>
+      <c r="D127" s="64" t="s">
+        <v>69</v>
+      </c>
+      <c r="E127" s="64" t="s">
+        <v>597</v>
+      </c>
+      <c r="F127" s="65"/>
+    </row>
+    <row r="128" spans="1:6" ht="150.75" thickBot="1">
+      <c r="A128" s="63">
+        <v>127</v>
+      </c>
+      <c r="B128" s="64" t="s">
+        <v>598</v>
+      </c>
+      <c r="C128" s="64"/>
+      <c r="D128" s="64" t="s">
+        <v>230</v>
+      </c>
+      <c r="E128" s="64" t="s">
+        <v>599</v>
+      </c>
+      <c r="F128" s="65"/>
+    </row>
+    <row r="129" spans="1:6" ht="45.75" thickBot="1">
+      <c r="A129" s="63">
+        <v>128</v>
+      </c>
+      <c r="B129" s="64" t="s">
+        <v>600</v>
+      </c>
+      <c r="C129" s="64"/>
+      <c r="D129" s="64" t="s">
+        <v>601</v>
+      </c>
+      <c r="E129" s="64" t="s">
+        <v>602</v>
+      </c>
+      <c r="F129" s="65"/>
+    </row>
+    <row r="130" spans="1:6" ht="135.75" thickBot="1">
+      <c r="A130" s="63">
+        <v>129</v>
+      </c>
+      <c r="B130" s="64" t="s">
+        <v>603</v>
+      </c>
+      <c r="C130" s="64"/>
+      <c r="D130" s="64" t="s">
+        <v>297</v>
+      </c>
+      <c r="E130" s="64" t="s">
+        <v>604</v>
+      </c>
+      <c r="F130" s="65"/>
+    </row>
+    <row r="131" spans="1:6" ht="150.75" thickBot="1">
+      <c r="A131" s="63">
+        <v>130</v>
+      </c>
+      <c r="B131" s="64" t="s">
+        <v>605</v>
+      </c>
+      <c r="C131" s="64"/>
+      <c r="D131" s="64" t="s">
+        <v>298</v>
+      </c>
+      <c r="E131" s="64" t="s">
+        <v>606</v>
+      </c>
+      <c r="F131" s="65"/>
+    </row>
+    <row r="132" spans="1:6" ht="150.75" thickBot="1">
+      <c r="A132" s="63">
+        <v>131</v>
+      </c>
+      <c r="B132" s="64" t="s">
+        <v>607</v>
+      </c>
+      <c r="C132" s="64"/>
+      <c r="D132" s="64" t="s">
+        <v>272</v>
+      </c>
+      <c r="E132" s="64" t="s">
+        <v>608</v>
+      </c>
+      <c r="F132" s="65"/>
+    </row>
+    <row r="133" spans="1:6" ht="150.75" thickBot="1">
+      <c r="A133" s="63">
+        <v>132</v>
+      </c>
+      <c r="B133" s="64" t="s">
+        <v>609</v>
+      </c>
+      <c r="C133" s="64"/>
+      <c r="D133" s="64" t="s">
+        <v>250</v>
+      </c>
+      <c r="E133" s="64" t="s">
+        <v>610</v>
+      </c>
+      <c r="F133" s="65"/>
+    </row>
+    <row r="134" spans="1:6" ht="135.75" thickBot="1">
+      <c r="A134" s="63">
+        <v>133</v>
+      </c>
+      <c r="B134" s="64" t="s">
+        <v>611</v>
+      </c>
+      <c r="C134" s="64"/>
+      <c r="D134" s="64" t="s">
+        <v>240</v>
+      </c>
+      <c r="E134" s="64" t="s">
+        <v>612</v>
+      </c>
+      <c r="F134" s="65"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:F84" xr:uid="{F040F6F6-EB53-40F8-B637-6D3CBDAE75E2}"/>

</xml_diff>